<commit_message>
Update references and familiar info
</commit_message>
<xml_diff>
--- a/front/src/assets/FORMATO_DE_VINCULACION.xlsx
+++ b/front/src/assets/FORMATO_DE_VINCULACION.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\femseapto\front\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B124EAF2-DF7F-4D4D-9FC5-602425B743BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{398C9827-55A0-482D-81D6-3FAEDB1C9E43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2470,12 +2470,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="469">
+  <cellXfs count="466">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2533,12 +2530,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2635,6 +2626,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="101" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="117" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -2707,66 +2704,78 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="111" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="94" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="95" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="96" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="94" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="95" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="96" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="99" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="100" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="101" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="111" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="94" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="95" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="96" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="94" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="95" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="96" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="99" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2833,9 +2842,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -2970,12 +2976,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="102" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="100" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3741,6 +3741,12 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -3762,9 +3768,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -3860,18 +3863,6 @@
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="101" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="117" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5013,7 +5004,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>514350</xdr:colOff>
+          <xdr:colOff>495300</xdr:colOff>
           <xdr:row>14</xdr:row>
           <xdr:rowOff>95250</xdr:rowOff>
         </xdr:to>
@@ -5424,7 +5415,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>38100</xdr:colOff>
+          <xdr:colOff>19050</xdr:colOff>
           <xdr:row>51</xdr:row>
           <xdr:rowOff>47625</xdr:rowOff>
         </xdr:to>
@@ -5596,7 +5587,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>19050</xdr:colOff>
+          <xdr:colOff>0</xdr:colOff>
           <xdr:row>52</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:to>
@@ -6111,8 +6102,8 @@
           <xdr:rowOff>209550</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>13</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>12</xdr:col>
+          <xdr:colOff>495300</xdr:colOff>
           <xdr:row>55</xdr:row>
           <xdr:rowOff>123825</xdr:rowOff>
         </xdr:to>
@@ -6627,8 +6618,8 @@
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>13</xdr:col>
-          <xdr:colOff>57150</xdr:colOff>
+          <xdr:col>12</xdr:col>
+          <xdr:colOff>552450</xdr:colOff>
           <xdr:row>57</xdr:row>
           <xdr:rowOff>133350</xdr:rowOff>
         </xdr:to>
@@ -7990,7 +7981,7 @@
   <dimension ref="A1:AJ164"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="Y8" sqref="Y8:AB8"/>
+      <selection activeCell="N42" sqref="N42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -8004,11 +7995,11 @@
     <col min="7" max="7" width="5.42578125" style="1" customWidth="1"/>
     <col min="8" max="8" width="4.28515625" style="1" customWidth="1"/>
     <col min="9" max="9" width="2.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="2.5703125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="2.85546875" style="1" customWidth="1"/>
     <col min="11" max="11" width="11.42578125" style="1" customWidth="1"/>
     <col min="12" max="12" width="6.28515625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="7.42578125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="6.140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="9.85546875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="8.85546875" style="1" customWidth="1"/>
     <col min="15" max="15" width="3.140625" style="1" customWidth="1"/>
     <col min="16" max="16" width="2" style="1" customWidth="1"/>
     <col min="17" max="17" width="6.42578125" style="1" customWidth="1"/>
@@ -8153,24 +8144,24 @@
     <row r="4" spans="1:34" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="254"/>
       <c r="B4" s="255"/>
-      <c r="C4" s="446" t="s">
+      <c r="C4" s="447" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="447"/>
-      <c r="E4" s="447"/>
-      <c r="F4" s="448"/>
-      <c r="G4" s="449"/>
-      <c r="H4" s="447"/>
-      <c r="I4" s="447"/>
-      <c r="J4" s="447"/>
-      <c r="K4" s="447"/>
-      <c r="L4" s="447"/>
-      <c r="M4" s="447"/>
-      <c r="N4" s="447"/>
-      <c r="O4" s="447"/>
-      <c r="P4" s="447"/>
-      <c r="Q4" s="447"/>
-      <c r="R4" s="448"/>
+      <c r="D4" s="448"/>
+      <c r="E4" s="448"/>
+      <c r="F4" s="449"/>
+      <c r="G4" s="450"/>
+      <c r="H4" s="448"/>
+      <c r="I4" s="448"/>
+      <c r="J4" s="448"/>
+      <c r="K4" s="448"/>
+      <c r="L4" s="448"/>
+      <c r="M4" s="448"/>
+      <c r="N4" s="448"/>
+      <c r="O4" s="448"/>
+      <c r="P4" s="448"/>
+      <c r="Q4" s="448"/>
+      <c r="R4" s="449"/>
       <c r="S4" s="264" t="s">
         <v>1</v>
       </c>
@@ -8182,15 +8173,15 @@
       <c r="Y4" s="264"/>
       <c r="Z4" s="264"/>
       <c r="AA4" s="264"/>
-      <c r="AB4" s="53" t="s">
+      <c r="AB4" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="AC4" s="53"/>
-      <c r="AD4" s="53"/>
-      <c r="AE4" s="53"/>
-      <c r="AF4" s="58"/>
-      <c r="AG4" s="58"/>
-      <c r="AH4" s="58"/>
+      <c r="AC4" s="50"/>
+      <c r="AD4" s="50"/>
+      <c r="AE4" s="50"/>
+      <c r="AF4" s="57"/>
+      <c r="AG4" s="57"/>
+      <c r="AH4" s="57"/>
     </row>
     <row r="5" spans="1:34" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="265" t="s">
@@ -8230,7 +8221,7 @@
       <c r="AG5" s="266"/>
       <c r="AH5" s="267"/>
     </row>
-    <row r="6" spans="1:34" s="34" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" s="31" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="277" t="s">
         <v>18</v>
       </c>
@@ -8278,29 +8269,29 @@
       </c>
       <c r="B7" s="269"/>
       <c r="C7" s="270"/>
-      <c r="D7" s="102"/>
-      <c r="E7" s="103"/>
-      <c r="F7" s="103"/>
-      <c r="G7" s="103"/>
-      <c r="H7" s="103"/>
-      <c r="I7" s="152"/>
+      <c r="D7" s="105"/>
+      <c r="E7" s="106"/>
+      <c r="F7" s="106"/>
+      <c r="G7" s="106"/>
+      <c r="H7" s="106"/>
+      <c r="I7" s="154"/>
       <c r="J7" s="280" t="s">
         <v>4</v>
       </c>
       <c r="K7" s="281"/>
       <c r="L7" s="290"/>
       <c r="M7" s="290"/>
-      <c r="N7" s="433" t="s">
+      <c r="N7" s="434" t="s">
         <v>113</v>
       </c>
-      <c r="O7" s="433"/>
-      <c r="P7" s="433"/>
-      <c r="Q7" s="434"/>
-      <c r="R7" s="149"/>
-      <c r="S7" s="149"/>
-      <c r="T7" s="149"/>
-      <c r="U7" s="149"/>
-      <c r="V7" s="150"/>
+      <c r="O7" s="434"/>
+      <c r="P7" s="434"/>
+      <c r="Q7" s="435"/>
+      <c r="R7" s="151"/>
+      <c r="S7" s="151"/>
+      <c r="T7" s="151"/>
+      <c r="U7" s="151"/>
+      <c r="V7" s="152"/>
       <c r="W7" s="172" t="s">
         <v>5</v>
       </c>
@@ -8316,12 +8307,12 @@
         <v>115</v>
       </c>
       <c r="AG7" s="282"/>
-      <c r="AH7" s="38" t="s">
+      <c r="AH7" s="35" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:34" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="23" t="s">
         <v>116</v>
       </c>
       <c r="B8" s="326" t="s">
@@ -8331,14 +8322,14 @@
       <c r="D8" s="328"/>
       <c r="E8" s="325"/>
       <c r="F8" s="319"/>
-      <c r="G8" s="103"/>
-      <c r="H8" s="103"/>
+      <c r="G8" s="106"/>
+      <c r="H8" s="106"/>
       <c r="I8" s="319"/>
       <c r="J8" s="319"/>
-      <c r="K8" s="103"/>
-      <c r="L8" s="103"/>
-      <c r="M8" s="103"/>
-      <c r="N8" s="152"/>
+      <c r="K8" s="106"/>
+      <c r="L8" s="106"/>
+      <c r="M8" s="106"/>
+      <c r="N8" s="154"/>
       <c r="O8" s="287" t="s">
         <v>118</v>
       </c>
@@ -8357,15 +8348,15 @@
       <c r="Z8" s="288"/>
       <c r="AA8" s="288"/>
       <c r="AB8" s="289"/>
-      <c r="AC8" s="102"/>
-      <c r="AD8" s="103"/>
-      <c r="AE8" s="103"/>
+      <c r="AC8" s="105"/>
+      <c r="AD8" s="106"/>
+      <c r="AE8" s="106"/>
       <c r="AF8" s="319"/>
       <c r="AG8" s="319"/>
-      <c r="AH8" s="104"/>
+      <c r="AH8" s="107"/>
     </row>
     <row r="9" spans="1:34" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="36" t="s">
         <v>120</v>
       </c>
       <c r="B9" s="321" t="s">
@@ -8387,12 +8378,12 @@
         <v>123</v>
       </c>
       <c r="L9" s="318"/>
-      <c r="M9" s="54" t="s">
+      <c r="M9" s="51" t="s">
         <v>110</v>
       </c>
-      <c r="N9" s="55"/>
-      <c r="O9" s="32"/>
-      <c r="P9" s="32"/>
+      <c r="N9" s="52"/>
+      <c r="O9" s="29"/>
+      <c r="P9" s="29"/>
       <c r="Q9" s="179" t="s">
         <v>167</v>
       </c>
@@ -8414,10 +8405,10 @@
         <v>121</v>
       </c>
       <c r="AG9" s="238"/>
-      <c r="AH9" s="27"/>
+      <c r="AH9" s="24"/>
     </row>
     <row r="10" spans="1:34" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="40" t="s">
+      <c r="A10" s="37" t="s">
         <v>126</v>
       </c>
       <c r="B10" s="315"/>
@@ -8427,41 +8418,41 @@
       <c r="F10" s="315"/>
       <c r="G10" s="315"/>
       <c r="H10" s="315"/>
-      <c r="I10" s="93" t="s">
+      <c r="I10" s="91" t="s">
         <v>127</v>
       </c>
-      <c r="J10" s="93"/>
-      <c r="K10" s="93"/>
+      <c r="J10" s="91"/>
+      <c r="K10" s="91"/>
       <c r="L10" s="316"/>
       <c r="M10" s="179"/>
       <c r="N10" s="179"/>
       <c r="O10" s="179"/>
       <c r="P10" s="179"/>
       <c r="Q10" s="179"/>
-      <c r="R10" s="93" t="s">
+      <c r="R10" s="91" t="s">
         <v>128</v>
       </c>
-      <c r="S10" s="93"/>
-      <c r="T10" s="93"/>
-      <c r="U10" s="93"/>
-      <c r="V10" s="93"/>
+      <c r="S10" s="91"/>
+      <c r="T10" s="91"/>
+      <c r="U10" s="91"/>
+      <c r="V10" s="91"/>
       <c r="W10" s="329"/>
-      <c r="X10" s="140"/>
-      <c r="Y10" s="140"/>
-      <c r="Z10" s="140"/>
-      <c r="AA10" s="140"/>
-      <c r="AB10" s="140"/>
-      <c r="AC10" s="140"/>
-      <c r="AD10" s="140"/>
+      <c r="X10" s="142"/>
+      <c r="Y10" s="142"/>
+      <c r="Z10" s="142"/>
+      <c r="AA10" s="142"/>
+      <c r="AB10" s="142"/>
+      <c r="AC10" s="142"/>
+      <c r="AD10" s="142"/>
       <c r="AE10" s="330"/>
-      <c r="AF10" s="68" t="s">
+      <c r="AF10" s="67" t="s">
         <v>129</v>
       </c>
-      <c r="AG10" s="70"/>
-      <c r="AH10" s="27"/>
+      <c r="AG10" s="69"/>
+      <c r="AH10" s="24"/>
     </row>
     <row r="11" spans="1:34" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="42" t="s">
+      <c r="A11" s="39" t="s">
         <v>130</v>
       </c>
       <c r="B11" s="331"/>
@@ -8474,10 +8465,10 @@
       <c r="I11" s="332"/>
       <c r="J11" s="332"/>
       <c r="K11" s="333"/>
-      <c r="L11" s="142" t="s">
+      <c r="L11" s="144" t="s">
         <v>131</v>
       </c>
-      <c r="M11" s="143"/>
+      <c r="M11" s="145"/>
       <c r="N11" s="317"/>
       <c r="O11" s="179"/>
       <c r="P11" s="179"/>
@@ -8493,188 +8484,188 @@
       <c r="X11" s="288"/>
       <c r="Y11" s="288"/>
       <c r="Z11" s="289"/>
-      <c r="AA11" s="102"/>
-      <c r="AB11" s="103"/>
-      <c r="AC11" s="103"/>
-      <c r="AD11" s="103"/>
-      <c r="AE11" s="103"/>
-      <c r="AF11" s="103"/>
-      <c r="AG11" s="103"/>
-      <c r="AH11" s="104"/>
+      <c r="AA11" s="105"/>
+      <c r="AB11" s="106"/>
+      <c r="AC11" s="106"/>
+      <c r="AD11" s="106"/>
+      <c r="AE11" s="106"/>
+      <c r="AF11" s="106"/>
+      <c r="AG11" s="106"/>
+      <c r="AH11" s="107"/>
     </row>
     <row r="12" spans="1:34" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="36" t="s">
+      <c r="A12" s="33" t="s">
         <v>132</v>
       </c>
-      <c r="B12" s="139"/>
-      <c r="C12" s="140"/>
-      <c r="D12" s="140"/>
-      <c r="E12" s="141"/>
-      <c r="F12" s="142" t="s">
+      <c r="B12" s="141"/>
+      <c r="C12" s="142"/>
+      <c r="D12" s="142"/>
+      <c r="E12" s="143"/>
+      <c r="F12" s="144" t="s">
         <v>133</v>
       </c>
-      <c r="G12" s="143"/>
-      <c r="H12" s="139"/>
-      <c r="I12" s="140"/>
-      <c r="J12" s="140"/>
-      <c r="K12" s="140"/>
-      <c r="L12" s="144"/>
-      <c r="M12" s="144"/>
-      <c r="N12" s="144"/>
-      <c r="O12" s="140"/>
-      <c r="P12" s="140"/>
-      <c r="Q12" s="141"/>
-      <c r="R12" s="94" t="s">
+      <c r="G12" s="145"/>
+      <c r="H12" s="141"/>
+      <c r="I12" s="142"/>
+      <c r="J12" s="142"/>
+      <c r="K12" s="142"/>
+      <c r="L12" s="146"/>
+      <c r="M12" s="146"/>
+      <c r="N12" s="146"/>
+      <c r="O12" s="142"/>
+      <c r="P12" s="142"/>
+      <c r="Q12" s="143"/>
+      <c r="R12" s="92" t="s">
         <v>134</v>
       </c>
-      <c r="S12" s="95"/>
-      <c r="T12" s="95"/>
-      <c r="U12" s="95"/>
-      <c r="V12" s="95"/>
-      <c r="W12" s="95"/>
-      <c r="X12" s="96"/>
-      <c r="Y12" s="139"/>
-      <c r="Z12" s="140"/>
-      <c r="AA12" s="140"/>
-      <c r="AB12" s="140"/>
-      <c r="AC12" s="140"/>
-      <c r="AD12" s="140"/>
-      <c r="AE12" s="140"/>
-      <c r="AF12" s="140"/>
-      <c r="AG12" s="140"/>
-      <c r="AH12" s="145"/>
+      <c r="S12" s="93"/>
+      <c r="T12" s="93"/>
+      <c r="U12" s="93"/>
+      <c r="V12" s="93"/>
+      <c r="W12" s="93"/>
+      <c r="X12" s="94"/>
+      <c r="Y12" s="141"/>
+      <c r="Z12" s="142"/>
+      <c r="AA12" s="142"/>
+      <c r="AB12" s="142"/>
+      <c r="AC12" s="142"/>
+      <c r="AD12" s="142"/>
+      <c r="AE12" s="142"/>
+      <c r="AF12" s="142"/>
+      <c r="AG12" s="142"/>
+      <c r="AH12" s="147"/>
     </row>
     <row r="13" spans="1:34" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="36" t="s">
+      <c r="A13" s="33" t="s">
         <v>135</v>
       </c>
-      <c r="B13" s="94"/>
-      <c r="C13" s="95"/>
-      <c r="D13" s="95"/>
-      <c r="E13" s="95"/>
-      <c r="F13" s="95"/>
-      <c r="G13" s="95"/>
-      <c r="H13" s="96"/>
-      <c r="I13" s="44" t="s">
+      <c r="B13" s="92"/>
+      <c r="C13" s="93"/>
+      <c r="D13" s="93"/>
+      <c r="E13" s="93"/>
+      <c r="F13" s="93"/>
+      <c r="G13" s="93"/>
+      <c r="H13" s="94"/>
+      <c r="I13" s="41" t="s">
         <v>137</v>
       </c>
-      <c r="J13" s="45"/>
-      <c r="K13" s="37"/>
-      <c r="L13" s="56" t="s">
+      <c r="J13" s="42"/>
+      <c r="K13" s="34"/>
+      <c r="L13" s="53" t="s">
         <v>138</v>
       </c>
-      <c r="M13" s="56"/>
-      <c r="N13" s="56"/>
-      <c r="O13" s="43"/>
-      <c r="P13" s="43"/>
-      <c r="Q13" s="57"/>
-      <c r="R13" s="164"/>
-      <c r="S13" s="165"/>
-      <c r="T13" s="165"/>
-      <c r="U13" s="165"/>
-      <c r="V13" s="165"/>
-      <c r="W13" s="165"/>
-      <c r="X13" s="165"/>
-      <c r="Y13" s="165"/>
-      <c r="Z13" s="165"/>
-      <c r="AA13" s="165"/>
-      <c r="AB13" s="165"/>
-      <c r="AC13" s="165"/>
-      <c r="AD13" s="165"/>
-      <c r="AE13" s="166"/>
-      <c r="AF13" s="44" t="s">
+      <c r="M13" s="53"/>
+      <c r="N13" s="53"/>
+      <c r="O13" s="40"/>
+      <c r="P13" s="40"/>
+      <c r="Q13" s="54"/>
+      <c r="R13" s="166"/>
+      <c r="S13" s="167"/>
+      <c r="T13" s="167"/>
+      <c r="U13" s="167"/>
+      <c r="V13" s="167"/>
+      <c r="W13" s="167"/>
+      <c r="X13" s="167"/>
+      <c r="Y13" s="167"/>
+      <c r="Z13" s="167"/>
+      <c r="AA13" s="167"/>
+      <c r="AB13" s="167"/>
+      <c r="AC13" s="167"/>
+      <c r="AD13" s="167"/>
+      <c r="AE13" s="168"/>
+      <c r="AF13" s="41" t="s">
         <v>136</v>
       </c>
-      <c r="AG13" s="139"/>
-      <c r="AH13" s="145"/>
+      <c r="AG13" s="141"/>
+      <c r="AH13" s="147"/>
     </row>
     <row r="14" spans="1:34" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="36" t="s">
+      <c r="A14" s="33" t="s">
         <v>139</v>
       </c>
-      <c r="B14" s="158" t="s">
+      <c r="B14" s="160" t="s">
         <v>140</v>
       </c>
-      <c r="C14" s="159"/>
-      <c r="D14" s="159"/>
-      <c r="E14" s="159"/>
-      <c r="F14" s="159"/>
-      <c r="G14" s="159"/>
-      <c r="H14" s="159"/>
-      <c r="I14" s="159"/>
-      <c r="J14" s="159"/>
-      <c r="K14" s="159"/>
-      <c r="L14" s="159"/>
-      <c r="M14" s="160"/>
-      <c r="N14" s="157" t="s">
+      <c r="C14" s="161"/>
+      <c r="D14" s="161"/>
+      <c r="E14" s="161"/>
+      <c r="F14" s="161"/>
+      <c r="G14" s="161"/>
+      <c r="H14" s="161"/>
+      <c r="I14" s="161"/>
+      <c r="J14" s="161"/>
+      <c r="K14" s="161"/>
+      <c r="L14" s="161"/>
+      <c r="M14" s="162"/>
+      <c r="N14" s="159" t="s">
         <v>9</v>
       </c>
-      <c r="O14" s="134"/>
-      <c r="P14" s="134"/>
-      <c r="Q14" s="135"/>
-      <c r="R14" s="139"/>
-      <c r="S14" s="140"/>
-      <c r="T14" s="140"/>
-      <c r="U14" s="140"/>
-      <c r="V14" s="140"/>
-      <c r="W14" s="140"/>
-      <c r="X14" s="140"/>
-      <c r="Y14" s="140"/>
-      <c r="Z14" s="140"/>
-      <c r="AA14" s="140"/>
-      <c r="AB14" s="140"/>
-      <c r="AC14" s="140"/>
-      <c r="AD14" s="140"/>
-      <c r="AE14" s="140"/>
-      <c r="AF14" s="140"/>
-      <c r="AG14" s="140"/>
-      <c r="AH14" s="145"/>
+      <c r="O14" s="136"/>
+      <c r="P14" s="136"/>
+      <c r="Q14" s="137"/>
+      <c r="R14" s="141"/>
+      <c r="S14" s="142"/>
+      <c r="T14" s="142"/>
+      <c r="U14" s="142"/>
+      <c r="V14" s="142"/>
+      <c r="W14" s="142"/>
+      <c r="X14" s="142"/>
+      <c r="Y14" s="142"/>
+      <c r="Z14" s="142"/>
+      <c r="AA14" s="142"/>
+      <c r="AB14" s="142"/>
+      <c r="AC14" s="142"/>
+      <c r="AD14" s="142"/>
+      <c r="AE14" s="142"/>
+      <c r="AF14" s="142"/>
+      <c r="AG14" s="142"/>
+      <c r="AH14" s="147"/>
     </row>
     <row r="15" spans="1:34" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="46" t="s">
+      <c r="A15" s="43" t="s">
         <v>92</v>
       </c>
-      <c r="B15" s="161"/>
-      <c r="C15" s="162"/>
-      <c r="D15" s="162"/>
-      <c r="E15" s="162"/>
-      <c r="F15" s="162"/>
-      <c r="G15" s="162"/>
-      <c r="H15" s="162"/>
-      <c r="I15" s="162"/>
-      <c r="J15" s="163"/>
-      <c r="K15" s="46" t="s">
+      <c r="B15" s="163"/>
+      <c r="C15" s="164"/>
+      <c r="D15" s="164"/>
+      <c r="E15" s="164"/>
+      <c r="F15" s="164"/>
+      <c r="G15" s="164"/>
+      <c r="H15" s="164"/>
+      <c r="I15" s="164"/>
+      <c r="J15" s="165"/>
+      <c r="K15" s="43" t="s">
         <v>93</v>
       </c>
-      <c r="L15" s="114"/>
-      <c r="M15" s="115"/>
-      <c r="N15" s="115"/>
-      <c r="O15" s="115"/>
-      <c r="P15" s="115"/>
-      <c r="Q15" s="116"/>
-      <c r="R15" s="117" t="s">
+      <c r="L15" s="117"/>
+      <c r="M15" s="118"/>
+      <c r="N15" s="118"/>
+      <c r="O15" s="118"/>
+      <c r="P15" s="118"/>
+      <c r="Q15" s="119"/>
+      <c r="R15" s="120" t="s">
         <v>141</v>
       </c>
-      <c r="S15" s="118"/>
-      <c r="T15" s="118"/>
-      <c r="U15" s="118"/>
-      <c r="V15" s="119"/>
-      <c r="W15" s="114"/>
-      <c r="X15" s="115"/>
-      <c r="Y15" s="115"/>
-      <c r="Z15" s="115"/>
-      <c r="AA15" s="115"/>
-      <c r="AB15" s="116"/>
+      <c r="S15" s="121"/>
+      <c r="T15" s="121"/>
+      <c r="U15" s="121"/>
+      <c r="V15" s="122"/>
+      <c r="W15" s="117"/>
+      <c r="X15" s="118"/>
+      <c r="Y15" s="118"/>
+      <c r="Z15" s="118"/>
+      <c r="AA15" s="118"/>
+      <c r="AB15" s="119"/>
       <c r="AC15" s="177" t="s">
         <v>130</v>
       </c>
       <c r="AD15" s="178"/>
       <c r="AE15" s="178"/>
       <c r="AF15" s="178"/>
-      <c r="AG15" s="91"/>
-      <c r="AH15" s="92"/>
-    </row>
-    <row r="16" spans="1:34" s="4" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AG15" s="88"/>
+      <c r="AH15" s="90"/>
+    </row>
+    <row r="16" spans="1:34" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="283" t="s">
         <v>10</v>
       </c>
@@ -8713,46 +8704,46 @@
       <c r="AH16" s="286"/>
     </row>
     <row r="17" spans="1:34" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="46" t="s">
+      <c r="A17" s="43" t="s">
         <v>142</v>
       </c>
-      <c r="B17" s="153"/>
-      <c r="C17" s="154"/>
-      <c r="D17" s="154"/>
-      <c r="E17" s="154"/>
-      <c r="F17" s="154"/>
-      <c r="G17" s="154"/>
-      <c r="H17" s="154"/>
-      <c r="I17" s="154"/>
-      <c r="J17" s="154"/>
-      <c r="K17" s="154"/>
-      <c r="L17" s="154"/>
-      <c r="M17" s="154"/>
-      <c r="N17" s="154"/>
-      <c r="O17" s="154"/>
-      <c r="P17" s="154"/>
-      <c r="Q17" s="154"/>
-      <c r="R17" s="154"/>
-      <c r="S17" s="154"/>
-      <c r="T17" s="154"/>
-      <c r="U17" s="154"/>
-      <c r="V17" s="154"/>
-      <c r="W17" s="154"/>
-      <c r="X17" s="155"/>
-      <c r="Y17" s="46" t="s">
+      <c r="B17" s="155"/>
+      <c r="C17" s="156"/>
+      <c r="D17" s="156"/>
+      <c r="E17" s="156"/>
+      <c r="F17" s="156"/>
+      <c r="G17" s="156"/>
+      <c r="H17" s="156"/>
+      <c r="I17" s="156"/>
+      <c r="J17" s="156"/>
+      <c r="K17" s="156"/>
+      <c r="L17" s="156"/>
+      <c r="M17" s="156"/>
+      <c r="N17" s="156"/>
+      <c r="O17" s="156"/>
+      <c r="P17" s="156"/>
+      <c r="Q17" s="156"/>
+      <c r="R17" s="156"/>
+      <c r="S17" s="156"/>
+      <c r="T17" s="156"/>
+      <c r="U17" s="156"/>
+      <c r="V17" s="156"/>
+      <c r="W17" s="156"/>
+      <c r="X17" s="157"/>
+      <c r="Y17" s="43" t="s">
         <v>136</v>
       </c>
-      <c r="Z17" s="46"/>
-      <c r="AA17" s="153"/>
-      <c r="AB17" s="154"/>
-      <c r="AC17" s="154"/>
-      <c r="AD17" s="154"/>
-      <c r="AE17" s="154"/>
-      <c r="AF17" s="154"/>
-      <c r="AG17" s="154"/>
-      <c r="AH17" s="156"/>
-    </row>
-    <row r="18" spans="1:34" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z17" s="43"/>
+      <c r="AA17" s="155"/>
+      <c r="AB17" s="156"/>
+      <c r="AC17" s="156"/>
+      <c r="AD17" s="156"/>
+      <c r="AE17" s="156"/>
+      <c r="AF17" s="156"/>
+      <c r="AG17" s="156"/>
+      <c r="AH17" s="158"/>
+    </row>
+    <row r="18" spans="1:34" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="191" t="s">
         <v>62</v>
       </c>
@@ -8791,266 +8782,266 @@
       <c r="AH18" s="195"/>
     </row>
     <row r="19" spans="1:34" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="41" t="s">
+      <c r="A19" s="38" t="s">
         <v>144</v>
       </c>
-      <c r="B19" s="123"/>
-      <c r="C19" s="124"/>
-      <c r="D19" s="124"/>
-      <c r="E19" s="124"/>
-      <c r="F19" s="125"/>
-      <c r="G19" s="120" t="s">
+      <c r="B19" s="126"/>
+      <c r="C19" s="103"/>
+      <c r="D19" s="103"/>
+      <c r="E19" s="103"/>
+      <c r="F19" s="127"/>
+      <c r="G19" s="123" t="s">
         <v>143</v>
       </c>
-      <c r="H19" s="121"/>
-      <c r="I19" s="121"/>
-      <c r="J19" s="122"/>
-      <c r="K19" s="71"/>
-      <c r="L19" s="72"/>
-      <c r="M19" s="73"/>
-      <c r="N19" s="120" t="s">
+      <c r="H19" s="124"/>
+      <c r="I19" s="124"/>
+      <c r="J19" s="125"/>
+      <c r="K19" s="70"/>
+      <c r="L19" s="71"/>
+      <c r="M19" s="72"/>
+      <c r="N19" s="123" t="s">
         <v>145</v>
       </c>
-      <c r="O19" s="121"/>
-      <c r="P19" s="121"/>
-      <c r="Q19" s="122"/>
-      <c r="R19" s="123"/>
-      <c r="S19" s="124"/>
-      <c r="T19" s="124"/>
-      <c r="U19" s="124"/>
-      <c r="V19" s="124"/>
-      <c r="W19" s="124"/>
-      <c r="X19" s="124"/>
-      <c r="Y19" s="124"/>
-      <c r="Z19" s="124"/>
-      <c r="AA19" s="124"/>
-      <c r="AB19" s="124"/>
-      <c r="AC19" s="124"/>
-      <c r="AD19" s="125"/>
-      <c r="AE19" s="126" t="s">
+      <c r="O19" s="124"/>
+      <c r="P19" s="124"/>
+      <c r="Q19" s="125"/>
+      <c r="R19" s="126"/>
+      <c r="S19" s="103"/>
+      <c r="T19" s="103"/>
+      <c r="U19" s="103"/>
+      <c r="V19" s="103"/>
+      <c r="W19" s="103"/>
+      <c r="X19" s="103"/>
+      <c r="Y19" s="103"/>
+      <c r="Z19" s="103"/>
+      <c r="AA19" s="103"/>
+      <c r="AB19" s="103"/>
+      <c r="AC19" s="103"/>
+      <c r="AD19" s="127"/>
+      <c r="AE19" s="128" t="s">
         <v>150</v>
       </c>
-      <c r="AF19" s="126"/>
-      <c r="AG19" s="71"/>
-      <c r="AH19" s="73"/>
+      <c r="AF19" s="128"/>
+      <c r="AG19" s="70"/>
+      <c r="AH19" s="72"/>
     </row>
     <row r="20" spans="1:34" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="36" t="s">
+      <c r="A20" s="33" t="s">
         <v>146</v>
       </c>
-      <c r="B20" s="79"/>
-      <c r="C20" s="81"/>
-      <c r="D20" s="133" t="s">
+      <c r="B20" s="78"/>
+      <c r="C20" s="80"/>
+      <c r="D20" s="135" t="s">
         <v>147</v>
       </c>
-      <c r="E20" s="134"/>
-      <c r="F20" s="134"/>
-      <c r="G20" s="135"/>
-      <c r="H20" s="136"/>
-      <c r="I20" s="137"/>
-      <c r="J20" s="137"/>
-      <c r="K20" s="138"/>
-      <c r="L20" s="146" t="s">
+      <c r="E20" s="136"/>
+      <c r="F20" s="136"/>
+      <c r="G20" s="137"/>
+      <c r="H20" s="138"/>
+      <c r="I20" s="139"/>
+      <c r="J20" s="139"/>
+      <c r="K20" s="140"/>
+      <c r="L20" s="148" t="s">
         <v>4</v>
       </c>
-      <c r="M20" s="147"/>
-      <c r="N20" s="148"/>
-      <c r="O20" s="149"/>
-      <c r="P20" s="149"/>
-      <c r="Q20" s="149"/>
-      <c r="R20" s="150"/>
-      <c r="S20" s="77" t="s">
+      <c r="M20" s="149"/>
+      <c r="N20" s="150"/>
+      <c r="O20" s="151"/>
+      <c r="P20" s="151"/>
+      <c r="Q20" s="151"/>
+      <c r="R20" s="152"/>
+      <c r="S20" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="T20" s="78"/>
-      <c r="U20" s="78"/>
-      <c r="V20" s="78"/>
-      <c r="W20" s="78"/>
-      <c r="X20" s="78"/>
-      <c r="Y20" s="151"/>
-      <c r="Z20" s="102"/>
-      <c r="AA20" s="103"/>
-      <c r="AB20" s="103"/>
-      <c r="AC20" s="103"/>
-      <c r="AD20" s="103"/>
-      <c r="AE20" s="152"/>
-      <c r="AF20" s="82" t="s">
+      <c r="T20" s="77"/>
+      <c r="U20" s="77"/>
+      <c r="V20" s="77"/>
+      <c r="W20" s="77"/>
+      <c r="X20" s="77"/>
+      <c r="Y20" s="153"/>
+      <c r="Z20" s="105"/>
+      <c r="AA20" s="106"/>
+      <c r="AB20" s="106"/>
+      <c r="AC20" s="106"/>
+      <c r="AD20" s="106"/>
+      <c r="AE20" s="154"/>
+      <c r="AF20" s="98" t="s">
         <v>115</v>
       </c>
-      <c r="AG20" s="83"/>
-      <c r="AH20" s="35"/>
+      <c r="AG20" s="99"/>
+      <c r="AH20" s="32"/>
     </row>
     <row r="21" spans="1:34" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="42" t="s">
+      <c r="A21" s="39" t="s">
         <v>148</v>
       </c>
-      <c r="B21" s="167"/>
-      <c r="C21" s="168"/>
-      <c r="D21" s="168"/>
-      <c r="E21" s="168"/>
-      <c r="F21" s="168"/>
-      <c r="G21" s="168"/>
-      <c r="H21" s="168"/>
-      <c r="I21" s="168"/>
-      <c r="J21" s="168"/>
-      <c r="K21" s="168"/>
-      <c r="L21" s="169"/>
-      <c r="M21" s="47" t="s">
+      <c r="B21" s="169"/>
+      <c r="C21" s="170"/>
+      <c r="D21" s="170"/>
+      <c r="E21" s="170"/>
+      <c r="F21" s="170"/>
+      <c r="G21" s="170"/>
+      <c r="H21" s="170"/>
+      <c r="I21" s="170"/>
+      <c r="J21" s="170"/>
+      <c r="K21" s="170"/>
+      <c r="L21" s="171"/>
+      <c r="M21" s="44" t="s">
         <v>149</v>
       </c>
-      <c r="N21" s="79"/>
-      <c r="O21" s="80"/>
-      <c r="P21" s="80"/>
-      <c r="Q21" s="80"/>
-      <c r="R21" s="80"/>
-      <c r="S21" s="80"/>
-      <c r="T21" s="81"/>
-      <c r="U21" s="77" t="s">
+      <c r="N21" s="78"/>
+      <c r="O21" s="79"/>
+      <c r="P21" s="79"/>
+      <c r="Q21" s="79"/>
+      <c r="R21" s="79"/>
+      <c r="S21" s="79"/>
+      <c r="T21" s="80"/>
+      <c r="U21" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="V21" s="78"/>
-      <c r="W21" s="78"/>
-      <c r="X21" s="78"/>
-      <c r="Y21" s="78"/>
-      <c r="Z21" s="97"/>
-      <c r="AA21" s="98"/>
-      <c r="AB21" s="98"/>
-      <c r="AC21" s="98"/>
-      <c r="AD21" s="99"/>
-      <c r="AE21" s="82" t="s">
+      <c r="V21" s="77"/>
+      <c r="W21" s="77"/>
+      <c r="X21" s="77"/>
+      <c r="Y21" s="77"/>
+      <c r="Z21" s="95"/>
+      <c r="AA21" s="96"/>
+      <c r="AB21" s="96"/>
+      <c r="AC21" s="96"/>
+      <c r="AD21" s="97"/>
+      <c r="AE21" s="98" t="s">
         <v>151</v>
       </c>
-      <c r="AF21" s="83"/>
+      <c r="AF21" s="99"/>
       <c r="AG21" s="100"/>
       <c r="AH21" s="101"/>
     </row>
     <row r="22" spans="1:34" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="41" t="s">
+      <c r="A22" s="38" t="s">
         <v>153</v>
       </c>
-      <c r="B22" s="84"/>
-      <c r="C22" s="80"/>
-      <c r="D22" s="80"/>
-      <c r="E22" s="80"/>
-      <c r="F22" s="80"/>
-      <c r="G22" s="80"/>
-      <c r="H22" s="80"/>
-      <c r="I22" s="80"/>
-      <c r="J22" s="80"/>
-      <c r="K22" s="80"/>
-      <c r="L22" s="81"/>
-      <c r="M22" s="47" t="s">
+      <c r="B22" s="81"/>
+      <c r="C22" s="79"/>
+      <c r="D22" s="79"/>
+      <c r="E22" s="79"/>
+      <c r="F22" s="79"/>
+      <c r="G22" s="79"/>
+      <c r="H22" s="79"/>
+      <c r="I22" s="79"/>
+      <c r="J22" s="79"/>
+      <c r="K22" s="79"/>
+      <c r="L22" s="80"/>
+      <c r="M22" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="N22" s="105"/>
-      <c r="O22" s="106"/>
-      <c r="P22" s="106"/>
-      <c r="Q22" s="106"/>
-      <c r="R22" s="106"/>
-      <c r="S22" s="106"/>
-      <c r="T22" s="107"/>
-      <c r="U22" s="77" t="s">
+      <c r="N22" s="108"/>
+      <c r="O22" s="109"/>
+      <c r="P22" s="109"/>
+      <c r="Q22" s="109"/>
+      <c r="R22" s="109"/>
+      <c r="S22" s="109"/>
+      <c r="T22" s="110"/>
+      <c r="U22" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="V22" s="78"/>
-      <c r="W22" s="78"/>
-      <c r="X22" s="78"/>
-      <c r="Y22" s="78"/>
-      <c r="Z22" s="97"/>
-      <c r="AA22" s="98"/>
-      <c r="AB22" s="98"/>
-      <c r="AC22" s="98"/>
-      <c r="AD22" s="99"/>
-      <c r="AE22" s="82" t="s">
+      <c r="V22" s="77"/>
+      <c r="W22" s="77"/>
+      <c r="X22" s="77"/>
+      <c r="Y22" s="77"/>
+      <c r="Z22" s="95"/>
+      <c r="AA22" s="96"/>
+      <c r="AB22" s="96"/>
+      <c r="AC22" s="96"/>
+      <c r="AD22" s="97"/>
+      <c r="AE22" s="98" t="s">
         <v>151</v>
       </c>
-      <c r="AF22" s="83"/>
+      <c r="AF22" s="99"/>
       <c r="AG22" s="100"/>
       <c r="AH22" s="101"/>
     </row>
     <row r="23" spans="1:34" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="41" t="s">
+      <c r="A23" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="B23" s="84"/>
-      <c r="C23" s="80"/>
-      <c r="D23" s="80"/>
-      <c r="E23" s="80"/>
-      <c r="F23" s="80"/>
-      <c r="G23" s="80"/>
-      <c r="H23" s="80"/>
-      <c r="I23" s="80"/>
-      <c r="J23" s="80"/>
-      <c r="K23" s="80"/>
-      <c r="L23" s="80"/>
-      <c r="M23" s="81"/>
-      <c r="N23" s="77" t="s">
+      <c r="B23" s="81"/>
+      <c r="C23" s="79"/>
+      <c r="D23" s="79"/>
+      <c r="E23" s="79"/>
+      <c r="F23" s="79"/>
+      <c r="G23" s="79"/>
+      <c r="H23" s="79"/>
+      <c r="I23" s="79"/>
+      <c r="J23" s="79"/>
+      <c r="K23" s="79"/>
+      <c r="L23" s="79"/>
+      <c r="M23" s="80"/>
+      <c r="N23" s="76" t="s">
         <v>155</v>
       </c>
-      <c r="O23" s="78"/>
-      <c r="P23" s="78"/>
-      <c r="Q23" s="79"/>
-      <c r="R23" s="80"/>
-      <c r="S23" s="80"/>
-      <c r="T23" s="80"/>
-      <c r="U23" s="80"/>
-      <c r="V23" s="80"/>
-      <c r="W23" s="80"/>
-      <c r="X23" s="80"/>
-      <c r="Y23" s="80"/>
-      <c r="Z23" s="80"/>
-      <c r="AA23" s="80"/>
-      <c r="AB23" s="80"/>
-      <c r="AC23" s="80"/>
-      <c r="AD23" s="80"/>
-      <c r="AE23" s="80"/>
-      <c r="AF23" s="81"/>
-      <c r="AG23" s="468" t="s">
+      <c r="O23" s="77"/>
+      <c r="P23" s="77"/>
+      <c r="Q23" s="78"/>
+      <c r="R23" s="79"/>
+      <c r="S23" s="79"/>
+      <c r="T23" s="79"/>
+      <c r="U23" s="79"/>
+      <c r="V23" s="79"/>
+      <c r="W23" s="79"/>
+      <c r="X23" s="79"/>
+      <c r="Y23" s="79"/>
+      <c r="Z23" s="79"/>
+      <c r="AA23" s="79"/>
+      <c r="AB23" s="79"/>
+      <c r="AC23" s="79"/>
+      <c r="AD23" s="79"/>
+      <c r="AE23" s="79"/>
+      <c r="AF23" s="80"/>
+      <c r="AG23" s="56" t="s">
         <v>152</v>
       </c>
-      <c r="AH23" s="466"/>
+      <c r="AH23" s="55"/>
     </row>
     <row r="24" spans="1:34" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="41" t="s">
+      <c r="A24" s="38" t="s">
         <v>156</v>
       </c>
-      <c r="B24" s="85"/>
-      <c r="C24" s="86"/>
-      <c r="D24" s="86"/>
-      <c r="E24" s="86"/>
-      <c r="F24" s="86"/>
-      <c r="G24" s="86"/>
-      <c r="H24" s="86"/>
-      <c r="I24" s="86"/>
-      <c r="J24" s="87"/>
-      <c r="K24" s="88" t="s">
+      <c r="B24" s="82"/>
+      <c r="C24" s="83"/>
+      <c r="D24" s="83"/>
+      <c r="E24" s="83"/>
+      <c r="F24" s="83"/>
+      <c r="G24" s="83"/>
+      <c r="H24" s="83"/>
+      <c r="I24" s="83"/>
+      <c r="J24" s="84"/>
+      <c r="K24" s="85" t="s">
         <v>157</v>
       </c>
-      <c r="L24" s="89"/>
-      <c r="M24" s="90"/>
-      <c r="N24" s="91"/>
-      <c r="O24" s="86"/>
-      <c r="P24" s="86"/>
-      <c r="Q24" s="86"/>
-      <c r="R24" s="86"/>
-      <c r="S24" s="86"/>
-      <c r="T24" s="86"/>
-      <c r="U24" s="86"/>
-      <c r="V24" s="86"/>
-      <c r="W24" s="86"/>
-      <c r="X24" s="86"/>
-      <c r="Y24" s="86"/>
-      <c r="Z24" s="86"/>
-      <c r="AA24" s="86"/>
-      <c r="AB24" s="86"/>
-      <c r="AC24" s="86"/>
-      <c r="AD24" s="86"/>
-      <c r="AE24" s="86"/>
-      <c r="AF24" s="86"/>
-      <c r="AG24" s="467"/>
-      <c r="AH24" s="92"/>
-    </row>
-    <row r="25" spans="1:34" s="4" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L24" s="86"/>
+      <c r="M24" s="87"/>
+      <c r="N24" s="88"/>
+      <c r="O24" s="83"/>
+      <c r="P24" s="83"/>
+      <c r="Q24" s="83"/>
+      <c r="R24" s="83"/>
+      <c r="S24" s="83"/>
+      <c r="T24" s="83"/>
+      <c r="U24" s="83"/>
+      <c r="V24" s="83"/>
+      <c r="W24" s="83"/>
+      <c r="X24" s="83"/>
+      <c r="Y24" s="83"/>
+      <c r="Z24" s="83"/>
+      <c r="AA24" s="83"/>
+      <c r="AB24" s="83"/>
+      <c r="AC24" s="83"/>
+      <c r="AD24" s="83"/>
+      <c r="AE24" s="83"/>
+      <c r="AF24" s="83"/>
+      <c r="AG24" s="89"/>
+      <c r="AH24" s="90"/>
+    </row>
+    <row r="25" spans="1:34" s="3" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="196" t="s">
         <v>63</v>
       </c>
@@ -9127,195 +9118,195 @@
       <c r="AH26" s="202"/>
     </row>
     <row r="27" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="22" t="s">
+      <c r="A27" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="146" t="s">
+      <c r="B27" s="148" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="147"/>
-      <c r="D27" s="147"/>
-      <c r="E27" s="147"/>
-      <c r="F27" s="147"/>
-      <c r="G27" s="147"/>
-      <c r="H27" s="147"/>
-      <c r="I27" s="147"/>
+      <c r="C27" s="149"/>
+      <c r="D27" s="149"/>
+      <c r="E27" s="149"/>
+      <c r="F27" s="149"/>
+      <c r="G27" s="149"/>
+      <c r="H27" s="149"/>
+      <c r="I27" s="149"/>
       <c r="J27" s="206"/>
-      <c r="K27" s="146" t="s">
+      <c r="K27" s="148" t="s">
         <v>30</v>
       </c>
-      <c r="L27" s="147"/>
-      <c r="M27" s="147"/>
-      <c r="N27" s="147"/>
-      <c r="O27" s="147"/>
-      <c r="P27" s="147"/>
-      <c r="Q27" s="147"/>
-      <c r="R27" s="147"/>
-      <c r="S27" s="147"/>
-      <c r="T27" s="147"/>
-      <c r="U27" s="147"/>
-      <c r="V27" s="147"/>
+      <c r="L27" s="149"/>
+      <c r="M27" s="149"/>
+      <c r="N27" s="149"/>
+      <c r="O27" s="149"/>
+      <c r="P27" s="149"/>
+      <c r="Q27" s="149"/>
+      <c r="R27" s="149"/>
+      <c r="S27" s="149"/>
+      <c r="T27" s="149"/>
+      <c r="U27" s="149"/>
+      <c r="V27" s="149"/>
       <c r="W27" s="206"/>
-      <c r="X27" s="146" t="s">
+      <c r="X27" s="148" t="s">
         <v>79</v>
       </c>
-      <c r="Y27" s="147"/>
-      <c r="Z27" s="147"/>
-      <c r="AA27" s="147"/>
-      <c r="AB27" s="147"/>
-      <c r="AC27" s="147"/>
-      <c r="AD27" s="147"/>
-      <c r="AE27" s="147"/>
-      <c r="AF27" s="147"/>
-      <c r="AG27" s="147"/>
+      <c r="Y27" s="149"/>
+      <c r="Z27" s="149"/>
+      <c r="AA27" s="149"/>
+      <c r="AB27" s="149"/>
+      <c r="AC27" s="149"/>
+      <c r="AD27" s="149"/>
+      <c r="AE27" s="149"/>
+      <c r="AF27" s="149"/>
+      <c r="AG27" s="149"/>
       <c r="AH27" s="207"/>
     </row>
     <row r="28" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="7"/>
-      <c r="B28" s="129"/>
-      <c r="C28" s="130"/>
-      <c r="D28" s="130"/>
-      <c r="E28" s="130"/>
-      <c r="F28" s="130"/>
-      <c r="G28" s="130"/>
-      <c r="H28" s="130"/>
-      <c r="I28" s="130"/>
-      <c r="J28" s="132"/>
-      <c r="K28" s="129"/>
-      <c r="L28" s="130"/>
-      <c r="M28" s="130"/>
-      <c r="N28" s="130"/>
-      <c r="O28" s="130"/>
-      <c r="P28" s="130"/>
-      <c r="Q28" s="130"/>
-      <c r="R28" s="130"/>
-      <c r="S28" s="130"/>
-      <c r="T28" s="130"/>
-      <c r="U28" s="130"/>
-      <c r="V28" s="130"/>
-      <c r="W28" s="132"/>
-      <c r="X28" s="129"/>
-      <c r="Y28" s="130"/>
-      <c r="Z28" s="130"/>
-      <c r="AA28" s="130"/>
-      <c r="AB28" s="130"/>
-      <c r="AC28" s="130"/>
-      <c r="AD28" s="130"/>
-      <c r="AE28" s="130"/>
-      <c r="AF28" s="130"/>
-      <c r="AG28" s="130"/>
-      <c r="AH28" s="131"/>
+      <c r="A28" s="6"/>
+      <c r="B28" s="131"/>
+      <c r="C28" s="132"/>
+      <c r="D28" s="132"/>
+      <c r="E28" s="132"/>
+      <c r="F28" s="132"/>
+      <c r="G28" s="132"/>
+      <c r="H28" s="132"/>
+      <c r="I28" s="132"/>
+      <c r="J28" s="134"/>
+      <c r="K28" s="131"/>
+      <c r="L28" s="132"/>
+      <c r="M28" s="132"/>
+      <c r="N28" s="132"/>
+      <c r="O28" s="132"/>
+      <c r="P28" s="132"/>
+      <c r="Q28" s="132"/>
+      <c r="R28" s="132"/>
+      <c r="S28" s="132"/>
+      <c r="T28" s="132"/>
+      <c r="U28" s="132"/>
+      <c r="V28" s="132"/>
+      <c r="W28" s="134"/>
+      <c r="X28" s="131"/>
+      <c r="Y28" s="132"/>
+      <c r="Z28" s="132"/>
+      <c r="AA28" s="132"/>
+      <c r="AB28" s="132"/>
+      <c r="AC28" s="132"/>
+      <c r="AD28" s="132"/>
+      <c r="AE28" s="132"/>
+      <c r="AF28" s="132"/>
+      <c r="AG28" s="132"/>
+      <c r="AH28" s="133"/>
     </row>
     <row r="29" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="7"/>
-      <c r="B29" s="129"/>
-      <c r="C29" s="130"/>
-      <c r="D29" s="130"/>
-      <c r="E29" s="130"/>
-      <c r="F29" s="130"/>
-      <c r="G29" s="130"/>
-      <c r="H29" s="130"/>
-      <c r="I29" s="130"/>
-      <c r="J29" s="132"/>
-      <c r="K29" s="129"/>
-      <c r="L29" s="130"/>
-      <c r="M29" s="130"/>
-      <c r="N29" s="130"/>
-      <c r="O29" s="130"/>
-      <c r="P29" s="130"/>
-      <c r="Q29" s="130"/>
-      <c r="R29" s="130"/>
-      <c r="S29" s="130"/>
-      <c r="T29" s="130"/>
-      <c r="U29" s="130"/>
-      <c r="V29" s="130"/>
-      <c r="W29" s="132"/>
-      <c r="X29" s="129"/>
-      <c r="Y29" s="130"/>
-      <c r="Z29" s="130"/>
-      <c r="AA29" s="130"/>
-      <c r="AB29" s="130"/>
-      <c r="AC29" s="130"/>
-      <c r="AD29" s="130"/>
-      <c r="AE29" s="130"/>
-      <c r="AF29" s="130"/>
-      <c r="AG29" s="130"/>
-      <c r="AH29" s="131"/>
+      <c r="A29" s="6"/>
+      <c r="B29" s="131"/>
+      <c r="C29" s="132"/>
+      <c r="D29" s="132"/>
+      <c r="E29" s="132"/>
+      <c r="F29" s="132"/>
+      <c r="G29" s="132"/>
+      <c r="H29" s="132"/>
+      <c r="I29" s="132"/>
+      <c r="J29" s="134"/>
+      <c r="K29" s="131"/>
+      <c r="L29" s="132"/>
+      <c r="M29" s="132"/>
+      <c r="N29" s="132"/>
+      <c r="O29" s="132"/>
+      <c r="P29" s="132"/>
+      <c r="Q29" s="132"/>
+      <c r="R29" s="132"/>
+      <c r="S29" s="132"/>
+      <c r="T29" s="132"/>
+      <c r="U29" s="132"/>
+      <c r="V29" s="132"/>
+      <c r="W29" s="134"/>
+      <c r="X29" s="131"/>
+      <c r="Y29" s="132"/>
+      <c r="Z29" s="132"/>
+      <c r="AA29" s="132"/>
+      <c r="AB29" s="132"/>
+      <c r="AC29" s="132"/>
+      <c r="AD29" s="132"/>
+      <c r="AE29" s="132"/>
+      <c r="AF29" s="132"/>
+      <c r="AG29" s="132"/>
+      <c r="AH29" s="133"/>
     </row>
     <row r="30" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="7"/>
-      <c r="B30" s="129"/>
-      <c r="C30" s="130"/>
-      <c r="D30" s="130"/>
-      <c r="E30" s="130"/>
-      <c r="F30" s="130"/>
-      <c r="G30" s="130"/>
-      <c r="H30" s="130"/>
-      <c r="I30" s="130"/>
-      <c r="J30" s="132"/>
-      <c r="K30" s="129"/>
-      <c r="L30" s="130"/>
-      <c r="M30" s="130"/>
-      <c r="N30" s="130"/>
-      <c r="O30" s="130"/>
-      <c r="P30" s="130"/>
-      <c r="Q30" s="130"/>
-      <c r="R30" s="130"/>
-      <c r="S30" s="130"/>
-      <c r="T30" s="130"/>
-      <c r="U30" s="130"/>
-      <c r="V30" s="130"/>
-      <c r="W30" s="132"/>
-      <c r="X30" s="129"/>
-      <c r="Y30" s="130"/>
-      <c r="Z30" s="130"/>
-      <c r="AA30" s="130"/>
-      <c r="AB30" s="130"/>
-      <c r="AC30" s="130"/>
-      <c r="AD30" s="130"/>
-      <c r="AE30" s="130"/>
-      <c r="AF30" s="130"/>
-      <c r="AG30" s="130"/>
-      <c r="AH30" s="131"/>
+      <c r="A30" s="6"/>
+      <c r="B30" s="131"/>
+      <c r="C30" s="132"/>
+      <c r="D30" s="132"/>
+      <c r="E30" s="132"/>
+      <c r="F30" s="132"/>
+      <c r="G30" s="132"/>
+      <c r="H30" s="132"/>
+      <c r="I30" s="132"/>
+      <c r="J30" s="134"/>
+      <c r="K30" s="131"/>
+      <c r="L30" s="132"/>
+      <c r="M30" s="132"/>
+      <c r="N30" s="132"/>
+      <c r="O30" s="132"/>
+      <c r="P30" s="132"/>
+      <c r="Q30" s="132"/>
+      <c r="R30" s="132"/>
+      <c r="S30" s="132"/>
+      <c r="T30" s="132"/>
+      <c r="U30" s="132"/>
+      <c r="V30" s="132"/>
+      <c r="W30" s="134"/>
+      <c r="X30" s="131"/>
+      <c r="Y30" s="132"/>
+      <c r="Z30" s="132"/>
+      <c r="AA30" s="132"/>
+      <c r="AB30" s="132"/>
+      <c r="AC30" s="132"/>
+      <c r="AD30" s="132"/>
+      <c r="AE30" s="132"/>
+      <c r="AF30" s="132"/>
+      <c r="AG30" s="132"/>
+      <c r="AH30" s="133"/>
     </row>
     <row r="31" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="7"/>
-      <c r="B31" s="129"/>
-      <c r="C31" s="130"/>
-      <c r="D31" s="130"/>
-      <c r="E31" s="130"/>
-      <c r="F31" s="130"/>
-      <c r="G31" s="130"/>
-      <c r="H31" s="130"/>
-      <c r="I31" s="130"/>
-      <c r="J31" s="132"/>
-      <c r="K31" s="129"/>
-      <c r="L31" s="130"/>
-      <c r="M31" s="130"/>
-      <c r="N31" s="130"/>
-      <c r="O31" s="130"/>
-      <c r="P31" s="130"/>
-      <c r="Q31" s="130"/>
-      <c r="R31" s="130"/>
-      <c r="S31" s="130"/>
-      <c r="T31" s="130"/>
-      <c r="U31" s="130"/>
-      <c r="V31" s="130"/>
-      <c r="W31" s="132"/>
-      <c r="X31" s="129"/>
-      <c r="Y31" s="130"/>
-      <c r="Z31" s="130"/>
-      <c r="AA31" s="130"/>
-      <c r="AB31" s="130"/>
-      <c r="AC31" s="130"/>
-      <c r="AD31" s="130"/>
-      <c r="AE31" s="130"/>
-      <c r="AF31" s="130"/>
-      <c r="AG31" s="130"/>
-      <c r="AH31" s="131"/>
+      <c r="A31" s="6"/>
+      <c r="B31" s="131"/>
+      <c r="C31" s="132"/>
+      <c r="D31" s="132"/>
+      <c r="E31" s="132"/>
+      <c r="F31" s="132"/>
+      <c r="G31" s="132"/>
+      <c r="H31" s="132"/>
+      <c r="I31" s="132"/>
+      <c r="J31" s="134"/>
+      <c r="K31" s="131"/>
+      <c r="L31" s="132"/>
+      <c r="M31" s="132"/>
+      <c r="N31" s="132"/>
+      <c r="O31" s="132"/>
+      <c r="P31" s="132"/>
+      <c r="Q31" s="132"/>
+      <c r="R31" s="132"/>
+      <c r="S31" s="132"/>
+      <c r="T31" s="132"/>
+      <c r="U31" s="132"/>
+      <c r="V31" s="132"/>
+      <c r="W31" s="134"/>
+      <c r="X31" s="131"/>
+      <c r="Y31" s="132"/>
+      <c r="Z31" s="132"/>
+      <c r="AA31" s="132"/>
+      <c r="AB31" s="132"/>
+      <c r="AC31" s="132"/>
+      <c r="AD31" s="132"/>
+      <c r="AE31" s="132"/>
+      <c r="AF31" s="132"/>
+      <c r="AG31" s="132"/>
+      <c r="AH31" s="133"/>
     </row>
     <row r="32" spans="1:34" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="8"/>
+      <c r="A32" s="7"/>
       <c r="B32" s="187"/>
       <c r="C32" s="188"/>
       <c r="D32" s="188"/>
@@ -9477,7 +9468,7 @@
       <c r="D36" s="238"/>
       <c r="E36" s="238"/>
       <c r="F36" s="238"/>
-      <c r="G36" s="464"/>
+      <c r="G36" s="465"/>
       <c r="H36" s="239"/>
       <c r="I36" s="239"/>
       <c r="J36" s="239"/>
@@ -9509,33 +9500,33 @@
       <c r="AH36" s="226"/>
     </row>
     <row r="37" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="93" t="s">
+      <c r="A37" s="91" t="s">
         <v>54</v>
       </c>
-      <c r="B37" s="93"/>
-      <c r="C37" s="93"/>
-      <c r="D37" s="93"/>
-      <c r="E37" s="93"/>
-      <c r="F37" s="93"/>
-      <c r="G37" s="71"/>
-      <c r="H37" s="72"/>
-      <c r="I37" s="72"/>
-      <c r="J37" s="72"/>
-      <c r="K37" s="72"/>
-      <c r="L37" s="73"/>
-      <c r="M37" s="459" t="s">
+      <c r="B37" s="91"/>
+      <c r="C37" s="91"/>
+      <c r="D37" s="91"/>
+      <c r="E37" s="91"/>
+      <c r="F37" s="91"/>
+      <c r="G37" s="70"/>
+      <c r="H37" s="71"/>
+      <c r="I37" s="71"/>
+      <c r="J37" s="71"/>
+      <c r="K37" s="71"/>
+      <c r="L37" s="72"/>
+      <c r="M37" s="460" t="s">
         <v>47</v>
       </c>
-      <c r="N37" s="460"/>
-      <c r="O37" s="460"/>
-      <c r="P37" s="460"/>
-      <c r="Q37" s="460"/>
-      <c r="R37" s="460"/>
-      <c r="S37" s="460"/>
-      <c r="T37" s="460"/>
-      <c r="U37" s="460"/>
-      <c r="V37" s="460"/>
-      <c r="W37" s="461"/>
+      <c r="N37" s="461"/>
+      <c r="O37" s="461"/>
+      <c r="P37" s="461"/>
+      <c r="Q37" s="461"/>
+      <c r="R37" s="461"/>
+      <c r="S37" s="461"/>
+      <c r="T37" s="461"/>
+      <c r="U37" s="461"/>
+      <c r="V37" s="461"/>
+      <c r="W37" s="462"/>
       <c r="X37" s="223"/>
       <c r="Y37" s="224"/>
       <c r="Z37" s="224"/>
@@ -9549,18 +9540,18 @@
       <c r="AH37" s="226"/>
     </row>
     <row r="38" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="93"/>
-      <c r="B38" s="93"/>
-      <c r="C38" s="93"/>
-      <c r="D38" s="93"/>
-      <c r="E38" s="93"/>
-      <c r="F38" s="93"/>
-      <c r="G38" s="71"/>
-      <c r="H38" s="72"/>
-      <c r="I38" s="72"/>
-      <c r="J38" s="72"/>
-      <c r="K38" s="72"/>
-      <c r="L38" s="73"/>
+      <c r="A38" s="91"/>
+      <c r="B38" s="91"/>
+      <c r="C38" s="91"/>
+      <c r="D38" s="91"/>
+      <c r="E38" s="91"/>
+      <c r="F38" s="91"/>
+      <c r="G38" s="70"/>
+      <c r="H38" s="71"/>
+      <c r="I38" s="71"/>
+      <c r="J38" s="71"/>
+      <c r="K38" s="71"/>
+      <c r="L38" s="72"/>
       <c r="M38" s="238" t="s">
         <v>48</v>
       </c>
@@ -9587,42 +9578,42 @@
       <c r="AH38" s="226"/>
     </row>
     <row r="39" spans="1:34" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="93"/>
-      <c r="B39" s="93"/>
-      <c r="C39" s="93"/>
-      <c r="D39" s="93"/>
-      <c r="E39" s="93"/>
-      <c r="F39" s="93"/>
-      <c r="G39" s="432"/>
-      <c r="H39" s="432"/>
-      <c r="I39" s="432"/>
-      <c r="J39" s="432"/>
-      <c r="K39" s="432"/>
-      <c r="L39" s="432"/>
-      <c r="M39" s="465" t="s">
+      <c r="A39" s="91"/>
+      <c r="B39" s="91"/>
+      <c r="C39" s="91"/>
+      <c r="D39" s="91"/>
+      <c r="E39" s="91"/>
+      <c r="F39" s="91"/>
+      <c r="G39" s="425"/>
+      <c r="H39" s="425"/>
+      <c r="I39" s="425"/>
+      <c r="J39" s="425"/>
+      <c r="K39" s="425"/>
+      <c r="L39" s="425"/>
+      <c r="M39" s="426" t="s">
         <v>49</v>
       </c>
-      <c r="N39" s="465"/>
-      <c r="O39" s="465"/>
-      <c r="P39" s="465"/>
-      <c r="Q39" s="465"/>
-      <c r="R39" s="465"/>
-      <c r="S39" s="465"/>
-      <c r="T39" s="465"/>
-      <c r="U39" s="465"/>
-      <c r="V39" s="465"/>
-      <c r="W39" s="465"/>
-      <c r="X39" s="425"/>
-      <c r="Y39" s="426"/>
-      <c r="Z39" s="426"/>
-      <c r="AA39" s="426"/>
-      <c r="AB39" s="426"/>
-      <c r="AC39" s="426"/>
-      <c r="AD39" s="426"/>
-      <c r="AE39" s="426"/>
-      <c r="AF39" s="427"/>
-      <c r="AG39" s="427"/>
-      <c r="AH39" s="428"/>
+      <c r="N39" s="426"/>
+      <c r="O39" s="426"/>
+      <c r="P39" s="426"/>
+      <c r="Q39" s="426"/>
+      <c r="R39" s="426"/>
+      <c r="S39" s="426"/>
+      <c r="T39" s="426"/>
+      <c r="U39" s="426"/>
+      <c r="V39" s="426"/>
+      <c r="W39" s="426"/>
+      <c r="X39" s="427"/>
+      <c r="Y39" s="428"/>
+      <c r="Z39" s="428"/>
+      <c r="AA39" s="428"/>
+      <c r="AB39" s="428"/>
+      <c r="AC39" s="428"/>
+      <c r="AD39" s="428"/>
+      <c r="AE39" s="428"/>
+      <c r="AF39" s="429"/>
+      <c r="AG39" s="429"/>
+      <c r="AH39" s="430"/>
     </row>
     <row r="40" spans="1:34" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="182" t="s">
@@ -9666,198 +9657,198 @@
       <c r="A41" s="233" t="s">
         <v>100</v>
       </c>
-      <c r="B41" s="128"/>
-      <c r="C41" s="128"/>
-      <c r="D41" s="128"/>
-      <c r="E41" s="128"/>
-      <c r="F41" s="128"/>
+      <c r="B41" s="130"/>
+      <c r="C41" s="130"/>
+      <c r="D41" s="130"/>
+      <c r="E41" s="130"/>
+      <c r="F41" s="130"/>
       <c r="G41" s="234"/>
-      <c r="H41" s="127" t="s">
+      <c r="H41" s="129" t="s">
         <v>101</v>
       </c>
-      <c r="I41" s="128"/>
+      <c r="I41" s="130"/>
       <c r="J41" s="234"/>
-      <c r="K41" s="127" t="s">
+      <c r="K41" s="129" t="s">
         <v>102</v>
       </c>
       <c r="L41" s="234"/>
-      <c r="M41" s="29" t="s">
+      <c r="M41" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="N41" s="29" t="s">
+      <c r="N41" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="O41" s="127" t="s">
+      <c r="O41" s="129" t="s">
         <v>105</v>
       </c>
-      <c r="P41" s="128"/>
-      <c r="Q41" s="128"/>
-      <c r="R41" s="128"/>
-      <c r="S41" s="128"/>
-      <c r="T41" s="128"/>
+      <c r="P41" s="130"/>
+      <c r="Q41" s="130"/>
+      <c r="R41" s="130"/>
+      <c r="S41" s="130"/>
+      <c r="T41" s="130"/>
       <c r="U41" s="234"/>
-      <c r="V41" s="127" t="s">
+      <c r="V41" s="129" t="s">
         <v>106</v>
       </c>
-      <c r="W41" s="128"/>
-      <c r="X41" s="128"/>
-      <c r="Y41" s="128"/>
-      <c r="Z41" s="128"/>
+      <c r="W41" s="130"/>
+      <c r="X41" s="130"/>
+      <c r="Y41" s="130"/>
+      <c r="Z41" s="130"/>
       <c r="AA41" s="234"/>
-      <c r="AB41" s="127" t="s">
+      <c r="AB41" s="129" t="s">
         <v>107</v>
       </c>
-      <c r="AC41" s="128"/>
-      <c r="AD41" s="128"/>
-      <c r="AE41" s="127" t="s">
+      <c r="AC41" s="130"/>
+      <c r="AD41" s="130"/>
+      <c r="AE41" s="129" t="s">
         <v>8</v>
       </c>
-      <c r="AF41" s="128"/>
-      <c r="AG41" s="128"/>
+      <c r="AF41" s="130"/>
+      <c r="AG41" s="130"/>
       <c r="AH41" s="343"/>
     </row>
     <row r="42" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="235"/>
-      <c r="B42" s="124"/>
-      <c r="C42" s="124"/>
-      <c r="D42" s="124"/>
-      <c r="E42" s="124"/>
-      <c r="F42" s="124"/>
-      <c r="G42" s="125"/>
-      <c r="H42" s="123"/>
-      <c r="I42" s="124"/>
-      <c r="J42" s="171"/>
-      <c r="K42" s="170"/>
-      <c r="L42" s="171"/>
-      <c r="M42" s="23"/>
-      <c r="N42" s="23"/>
-      <c r="O42" s="170"/>
-      <c r="P42" s="124"/>
-      <c r="Q42" s="124"/>
-      <c r="R42" s="124"/>
-      <c r="S42" s="124"/>
-      <c r="T42" s="124"/>
-      <c r="U42" s="171"/>
-      <c r="V42" s="170"/>
-      <c r="W42" s="124"/>
-      <c r="X42" s="124"/>
-      <c r="Y42" s="124"/>
-      <c r="Z42" s="124"/>
-      <c r="AA42" s="171"/>
-      <c r="AB42" s="24"/>
-      <c r="AC42" s="2"/>
-      <c r="AD42" s="25"/>
-      <c r="AE42" s="170"/>
-      <c r="AF42" s="124"/>
-      <c r="AG42" s="124"/>
+      <c r="B42" s="103"/>
+      <c r="C42" s="103"/>
+      <c r="D42" s="103"/>
+      <c r="E42" s="103"/>
+      <c r="F42" s="103"/>
+      <c r="G42" s="127"/>
+      <c r="H42" s="126"/>
+      <c r="I42" s="103"/>
+      <c r="J42" s="104"/>
+      <c r="K42" s="102"/>
+      <c r="L42" s="104"/>
+      <c r="M42" s="22"/>
+      <c r="N42" s="22"/>
+      <c r="O42" s="102"/>
+      <c r="P42" s="103"/>
+      <c r="Q42" s="103"/>
+      <c r="R42" s="103"/>
+      <c r="S42" s="103"/>
+      <c r="T42" s="103"/>
+      <c r="U42" s="104"/>
+      <c r="V42" s="102"/>
+      <c r="W42" s="103"/>
+      <c r="X42" s="103"/>
+      <c r="Y42" s="103"/>
+      <c r="Z42" s="103"/>
+      <c r="AA42" s="104"/>
+      <c r="AB42" s="102"/>
+      <c r="AC42" s="103"/>
+      <c r="AD42" s="104"/>
+      <c r="AE42" s="102"/>
+      <c r="AF42" s="103"/>
+      <c r="AG42" s="103"/>
       <c r="AH42" s="232"/>
     </row>
     <row r="43" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="235"/>
-      <c r="B43" s="124"/>
-      <c r="C43" s="124"/>
-      <c r="D43" s="124"/>
-      <c r="E43" s="124"/>
-      <c r="F43" s="124"/>
-      <c r="G43" s="171"/>
-      <c r="H43" s="170"/>
-      <c r="I43" s="124"/>
-      <c r="J43" s="171"/>
-      <c r="K43" s="170"/>
-      <c r="L43" s="171"/>
-      <c r="M43" s="23"/>
-      <c r="N43" s="23"/>
-      <c r="O43" s="170"/>
-      <c r="P43" s="124"/>
-      <c r="Q43" s="124"/>
-      <c r="R43" s="124"/>
-      <c r="S43" s="124"/>
-      <c r="T43" s="124"/>
-      <c r="U43" s="171"/>
-      <c r="V43" s="170"/>
-      <c r="W43" s="124"/>
-      <c r="X43" s="124"/>
-      <c r="Y43" s="124"/>
-      <c r="Z43" s="124"/>
-      <c r="AA43" s="171"/>
-      <c r="AB43" s="170"/>
-      <c r="AC43" s="124"/>
-      <c r="AD43" s="171"/>
-      <c r="AE43" s="170"/>
-      <c r="AF43" s="124"/>
-      <c r="AG43" s="124"/>
+      <c r="B43" s="103"/>
+      <c r="C43" s="103"/>
+      <c r="D43" s="103"/>
+      <c r="E43" s="103"/>
+      <c r="F43" s="103"/>
+      <c r="G43" s="104"/>
+      <c r="H43" s="102"/>
+      <c r="I43" s="103"/>
+      <c r="J43" s="104"/>
+      <c r="K43" s="102"/>
+      <c r="L43" s="104"/>
+      <c r="M43" s="22"/>
+      <c r="N43" s="22"/>
+      <c r="O43" s="102"/>
+      <c r="P43" s="103"/>
+      <c r="Q43" s="103"/>
+      <c r="R43" s="103"/>
+      <c r="S43" s="103"/>
+      <c r="T43" s="103"/>
+      <c r="U43" s="104"/>
+      <c r="V43" s="102"/>
+      <c r="W43" s="103"/>
+      <c r="X43" s="103"/>
+      <c r="Y43" s="103"/>
+      <c r="Z43" s="103"/>
+      <c r="AA43" s="104"/>
+      <c r="AB43" s="102"/>
+      <c r="AC43" s="103"/>
+      <c r="AD43" s="104"/>
+      <c r="AE43" s="102"/>
+      <c r="AF43" s="103"/>
+      <c r="AG43" s="103"/>
       <c r="AH43" s="232"/>
     </row>
     <row r="44" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="235"/>
-      <c r="B44" s="124"/>
-      <c r="C44" s="124"/>
-      <c r="D44" s="124"/>
-      <c r="E44" s="124"/>
-      <c r="F44" s="124"/>
-      <c r="G44" s="171"/>
-      <c r="H44" s="170"/>
-      <c r="I44" s="124"/>
-      <c r="J44" s="171"/>
-      <c r="K44" s="170"/>
-      <c r="L44" s="171"/>
-      <c r="M44" s="23"/>
-      <c r="N44" s="23"/>
-      <c r="O44" s="170"/>
-      <c r="P44" s="124"/>
-      <c r="Q44" s="124"/>
-      <c r="R44" s="124"/>
-      <c r="S44" s="124"/>
-      <c r="T44" s="124"/>
-      <c r="U44" s="171"/>
-      <c r="V44" s="170"/>
-      <c r="W44" s="124"/>
-      <c r="X44" s="124"/>
-      <c r="Y44" s="124"/>
-      <c r="Z44" s="124"/>
-      <c r="AA44" s="171"/>
-      <c r="AB44" s="170"/>
-      <c r="AC44" s="124"/>
-      <c r="AD44" s="171"/>
-      <c r="AE44" s="170"/>
-      <c r="AF44" s="124"/>
-      <c r="AG44" s="124"/>
+      <c r="B44" s="103"/>
+      <c r="C44" s="103"/>
+      <c r="D44" s="103"/>
+      <c r="E44" s="103"/>
+      <c r="F44" s="103"/>
+      <c r="G44" s="104"/>
+      <c r="H44" s="102"/>
+      <c r="I44" s="103"/>
+      <c r="J44" s="104"/>
+      <c r="K44" s="102"/>
+      <c r="L44" s="104"/>
+      <c r="M44" s="22"/>
+      <c r="N44" s="22"/>
+      <c r="O44" s="102"/>
+      <c r="P44" s="103"/>
+      <c r="Q44" s="103"/>
+      <c r="R44" s="103"/>
+      <c r="S44" s="103"/>
+      <c r="T44" s="103"/>
+      <c r="U44" s="104"/>
+      <c r="V44" s="102"/>
+      <c r="W44" s="103"/>
+      <c r="X44" s="103"/>
+      <c r="Y44" s="103"/>
+      <c r="Z44" s="103"/>
+      <c r="AA44" s="104"/>
+      <c r="AB44" s="102"/>
+      <c r="AC44" s="103"/>
+      <c r="AD44" s="104"/>
+      <c r="AE44" s="102"/>
+      <c r="AF44" s="103"/>
+      <c r="AG44" s="103"/>
       <c r="AH44" s="232"/>
     </row>
     <row r="45" spans="1:34" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="236"/>
-      <c r="B45" s="115"/>
-      <c r="C45" s="115"/>
-      <c r="D45" s="115"/>
-      <c r="E45" s="115"/>
-      <c r="F45" s="115"/>
-      <c r="G45" s="116"/>
-      <c r="H45" s="114"/>
-      <c r="I45" s="115"/>
-      <c r="J45" s="116"/>
-      <c r="K45" s="114"/>
-      <c r="L45" s="116"/>
-      <c r="M45" s="28"/>
-      <c r="N45" s="28"/>
-      <c r="O45" s="114"/>
-      <c r="P45" s="115"/>
-      <c r="Q45" s="115"/>
-      <c r="R45" s="115"/>
-      <c r="S45" s="115"/>
-      <c r="T45" s="115"/>
-      <c r="U45" s="116"/>
-      <c r="V45" s="114"/>
-      <c r="W45" s="115"/>
-      <c r="X45" s="115"/>
-      <c r="Y45" s="115"/>
-      <c r="Z45" s="115"/>
-      <c r="AA45" s="116"/>
-      <c r="AB45" s="114"/>
-      <c r="AC45" s="115"/>
-      <c r="AD45" s="116"/>
-      <c r="AE45" s="114"/>
-      <c r="AF45" s="115"/>
-      <c r="AG45" s="115"/>
+      <c r="B45" s="118"/>
+      <c r="C45" s="118"/>
+      <c r="D45" s="118"/>
+      <c r="E45" s="118"/>
+      <c r="F45" s="118"/>
+      <c r="G45" s="119"/>
+      <c r="H45" s="117"/>
+      <c r="I45" s="118"/>
+      <c r="J45" s="119"/>
+      <c r="K45" s="117"/>
+      <c r="L45" s="119"/>
+      <c r="M45" s="25"/>
+      <c r="N45" s="25"/>
+      <c r="O45" s="117"/>
+      <c r="P45" s="118"/>
+      <c r="Q45" s="118"/>
+      <c r="R45" s="118"/>
+      <c r="S45" s="118"/>
+      <c r="T45" s="118"/>
+      <c r="U45" s="119"/>
+      <c r="V45" s="117"/>
+      <c r="W45" s="118"/>
+      <c r="X45" s="118"/>
+      <c r="Y45" s="118"/>
+      <c r="Z45" s="118"/>
+      <c r="AA45" s="119"/>
+      <c r="AB45" s="117"/>
+      <c r="AC45" s="118"/>
+      <c r="AD45" s="119"/>
+      <c r="AE45" s="117"/>
+      <c r="AF45" s="118"/>
+      <c r="AG45" s="118"/>
       <c r="AH45" s="344"/>
     </row>
     <row r="46" spans="1:34" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -9911,7 +9902,7 @@
       <c r="H47" s="337"/>
       <c r="I47" s="337"/>
       <c r="J47" s="338"/>
-      <c r="K47" s="48" t="s">
+      <c r="K47" s="45" t="s">
         <v>31</v>
       </c>
       <c r="L47" s="339" t="s">
@@ -9946,16 +9937,16 @@
     </row>
     <row r="48" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="235"/>
-      <c r="B48" s="124"/>
-      <c r="C48" s="124"/>
-      <c r="D48" s="124"/>
-      <c r="E48" s="124"/>
-      <c r="F48" s="124"/>
-      <c r="G48" s="124"/>
-      <c r="H48" s="124"/>
-      <c r="I48" s="124"/>
-      <c r="J48" s="171"/>
-      <c r="K48" s="3"/>
+      <c r="B48" s="103"/>
+      <c r="C48" s="103"/>
+      <c r="D48" s="103"/>
+      <c r="E48" s="103"/>
+      <c r="F48" s="103"/>
+      <c r="G48" s="103"/>
+      <c r="H48" s="103"/>
+      <c r="I48" s="103"/>
+      <c r="J48" s="104"/>
+      <c r="K48" s="2"/>
       <c r="L48" s="240"/>
       <c r="M48" s="240"/>
       <c r="N48" s="240"/>
@@ -9982,16 +9973,16 @@
     </row>
     <row r="49" spans="1:35" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="236"/>
-      <c r="B49" s="115"/>
-      <c r="C49" s="115"/>
-      <c r="D49" s="115"/>
-      <c r="E49" s="115"/>
-      <c r="F49" s="115"/>
-      <c r="G49" s="115"/>
-      <c r="H49" s="115"/>
-      <c r="I49" s="115"/>
-      <c r="J49" s="116"/>
-      <c r="K49" s="3"/>
+      <c r="B49" s="118"/>
+      <c r="C49" s="118"/>
+      <c r="D49" s="118"/>
+      <c r="E49" s="118"/>
+      <c r="F49" s="118"/>
+      <c r="G49" s="118"/>
+      <c r="H49" s="118"/>
+      <c r="I49" s="118"/>
+      <c r="J49" s="119"/>
+      <c r="K49" s="2"/>
       <c r="L49" s="240"/>
       <c r="M49" s="240"/>
       <c r="N49" s="240"/>
@@ -10067,83 +10058,83 @@
       <c r="H51" s="238"/>
       <c r="I51" s="238"/>
       <c r="J51" s="238"/>
-      <c r="K51" s="49" t="s">
+      <c r="K51" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="L51" s="59"/>
-      <c r="M51" s="60"/>
-      <c r="N51" s="60"/>
-      <c r="O51" s="61"/>
-      <c r="P51" s="63" t="s">
+      <c r="L51" s="58"/>
+      <c r="M51" s="59"/>
+      <c r="N51" s="59"/>
+      <c r="O51" s="60"/>
+      <c r="P51" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="Q51" s="64"/>
-      <c r="R51" s="64"/>
-      <c r="S51" s="64"/>
-      <c r="T51" s="64"/>
-      <c r="U51" s="64"/>
-      <c r="V51" s="64"/>
-      <c r="W51" s="64"/>
-      <c r="X51" s="65"/>
-      <c r="Y51" s="59"/>
-      <c r="Z51" s="60"/>
-      <c r="AA51" s="60"/>
-      <c r="AB51" s="60"/>
-      <c r="AC51" s="60"/>
-      <c r="AD51" s="60"/>
-      <c r="AE51" s="60"/>
-      <c r="AF51" s="60"/>
-      <c r="AG51" s="60"/>
-      <c r="AH51" s="62"/>
+      <c r="Q51" s="63"/>
+      <c r="R51" s="63"/>
+      <c r="S51" s="63"/>
+      <c r="T51" s="63"/>
+      <c r="U51" s="63"/>
+      <c r="V51" s="63"/>
+      <c r="W51" s="63"/>
+      <c r="X51" s="64"/>
+      <c r="Y51" s="58"/>
+      <c r="Z51" s="59"/>
+      <c r="AA51" s="59"/>
+      <c r="AB51" s="59"/>
+      <c r="AC51" s="59"/>
+      <c r="AD51" s="59"/>
+      <c r="AE51" s="59"/>
+      <c r="AF51" s="59"/>
+      <c r="AG51" s="59"/>
+      <c r="AH51" s="61"/>
     </row>
     <row r="52" spans="1:35" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="429" t="s">
+      <c r="A52" s="431" t="s">
         <v>32</v>
       </c>
-      <c r="B52" s="430"/>
-      <c r="C52" s="430"/>
-      <c r="D52" s="430"/>
-      <c r="E52" s="430"/>
-      <c r="F52" s="431"/>
-      <c r="G52" s="462"/>
-      <c r="H52" s="463"/>
-      <c r="I52" s="463"/>
-      <c r="J52" s="463"/>
-      <c r="K52" s="50" t="s">
+      <c r="B52" s="432"/>
+      <c r="C52" s="432"/>
+      <c r="D52" s="432"/>
+      <c r="E52" s="432"/>
+      <c r="F52" s="433"/>
+      <c r="G52" s="463"/>
+      <c r="H52" s="464"/>
+      <c r="I52" s="464"/>
+      <c r="J52" s="464"/>
+      <c r="K52" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="L52" s="66" t="s">
+      <c r="L52" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="M52" s="67"/>
-      <c r="N52" s="58"/>
-      <c r="O52" s="58"/>
-      <c r="P52" s="58"/>
-      <c r="Q52" s="58"/>
-      <c r="R52" s="58"/>
-      <c r="S52" s="68" t="s">
+      <c r="M52" s="66"/>
+      <c r="N52" s="57"/>
+      <c r="O52" s="57"/>
+      <c r="P52" s="57"/>
+      <c r="Q52" s="57"/>
+      <c r="R52" s="57"/>
+      <c r="S52" s="67" t="s">
         <v>35</v>
       </c>
-      <c r="T52" s="69"/>
-      <c r="U52" s="69"/>
-      <c r="V52" s="69"/>
-      <c r="W52" s="70"/>
-      <c r="X52" s="71"/>
-      <c r="Y52" s="72"/>
-      <c r="Z52" s="73"/>
-      <c r="AA52" s="68" t="s">
+      <c r="T52" s="68"/>
+      <c r="U52" s="68"/>
+      <c r="V52" s="68"/>
+      <c r="W52" s="69"/>
+      <c r="X52" s="70"/>
+      <c r="Y52" s="71"/>
+      <c r="Z52" s="72"/>
+      <c r="AA52" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="AB52" s="69"/>
-      <c r="AC52" s="70"/>
-      <c r="AD52" s="74"/>
-      <c r="AE52" s="75"/>
-      <c r="AF52" s="76"/>
-      <c r="AG52" s="50" t="s">
+      <c r="AB52" s="68"/>
+      <c r="AC52" s="69"/>
+      <c r="AD52" s="73"/>
+      <c r="AE52" s="74"/>
+      <c r="AF52" s="75"/>
+      <c r="AG52" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="AH52" s="51"/>
-      <c r="AI52" s="52"/>
+      <c r="AH52" s="48"/>
+      <c r="AI52" s="49"/>
     </row>
     <row r="53" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A53" s="182" t="s">
@@ -10245,37 +10236,37 @@
       <c r="O55" s="240"/>
       <c r="P55" s="240"/>
       <c r="Q55" s="240"/>
-      <c r="R55" s="170"/>
-      <c r="S55" s="124"/>
-      <c r="T55" s="124"/>
-      <c r="U55" s="124"/>
-      <c r="V55" s="124"/>
-      <c r="W55" s="124"/>
-      <c r="X55" s="124"/>
-      <c r="Y55" s="124"/>
-      <c r="Z55" s="124"/>
-      <c r="AA55" s="124"/>
-      <c r="AB55" s="124"/>
-      <c r="AC55" s="124"/>
-      <c r="AD55" s="124"/>
-      <c r="AE55" s="124"/>
-      <c r="AF55" s="124"/>
-      <c r="AG55" s="124"/>
+      <c r="R55" s="102"/>
+      <c r="S55" s="103"/>
+      <c r="T55" s="103"/>
+      <c r="U55" s="103"/>
+      <c r="V55" s="103"/>
+      <c r="W55" s="103"/>
+      <c r="X55" s="103"/>
+      <c r="Y55" s="103"/>
+      <c r="Z55" s="103"/>
+      <c r="AA55" s="103"/>
+      <c r="AB55" s="103"/>
+      <c r="AC55" s="103"/>
+      <c r="AD55" s="103"/>
+      <c r="AE55" s="103"/>
+      <c r="AF55" s="103"/>
+      <c r="AG55" s="103"/>
       <c r="AH55" s="232"/>
     </row>
     <row r="56" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="302" t="s">
         <v>59</v>
       </c>
-      <c r="B56" s="165"/>
-      <c r="C56" s="165"/>
-      <c r="D56" s="165"/>
-      <c r="E56" s="165"/>
-      <c r="F56" s="165"/>
-      <c r="G56" s="165"/>
-      <c r="H56" s="165"/>
-      <c r="I56" s="165"/>
-      <c r="J56" s="166"/>
+      <c r="B56" s="167"/>
+      <c r="C56" s="167"/>
+      <c r="D56" s="167"/>
+      <c r="E56" s="167"/>
+      <c r="F56" s="167"/>
+      <c r="G56" s="167"/>
+      <c r="H56" s="167"/>
+      <c r="I56" s="167"/>
+      <c r="J56" s="168"/>
       <c r="K56" s="299" t="s">
         <v>60</v>
       </c>
@@ -10288,21 +10279,21 @@
       <c r="R56" s="300" t="s">
         <v>61</v>
       </c>
-      <c r="S56" s="165"/>
-      <c r="T56" s="165"/>
-      <c r="U56" s="165"/>
-      <c r="V56" s="165"/>
-      <c r="W56" s="165"/>
-      <c r="X56" s="165"/>
-      <c r="Y56" s="165"/>
-      <c r="Z56" s="165"/>
-      <c r="AA56" s="165"/>
-      <c r="AB56" s="165"/>
-      <c r="AC56" s="165"/>
-      <c r="AD56" s="165"/>
-      <c r="AE56" s="165"/>
-      <c r="AF56" s="165"/>
-      <c r="AG56" s="165"/>
+      <c r="S56" s="167"/>
+      <c r="T56" s="167"/>
+      <c r="U56" s="167"/>
+      <c r="V56" s="167"/>
+      <c r="W56" s="167"/>
+      <c r="X56" s="167"/>
+      <c r="Y56" s="167"/>
+      <c r="Z56" s="167"/>
+      <c r="AA56" s="167"/>
+      <c r="AB56" s="167"/>
+      <c r="AC56" s="167"/>
+      <c r="AD56" s="167"/>
+      <c r="AE56" s="167"/>
+      <c r="AF56" s="167"/>
+      <c r="AG56" s="167"/>
       <c r="AH56" s="301"/>
     </row>
     <row r="57" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -10417,7 +10408,7 @@
       <c r="AG59" s="293"/>
       <c r="AH59" s="294"/>
     </row>
-    <row r="60" spans="1:35" s="12" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:35" s="11" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="308" t="s">
         <v>166</v>
       </c>
@@ -10874,7 +10865,7 @@
       <c r="AF71" s="365"/>
       <c r="AG71" s="365"/>
       <c r="AH71" s="366"/>
-      <c r="AI71" s="5"/>
+      <c r="AI71" s="4"/>
     </row>
     <row r="72" spans="1:35" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="208" t="s">
@@ -10916,7 +10907,7 @@
       </c>
       <c r="AD72" s="209"/>
       <c r="AE72" s="209"/>
-      <c r="AF72" s="31"/>
+      <c r="AF72" s="28"/>
       <c r="AG72" s="314"/>
       <c r="AH72" s="314"/>
     </row>
@@ -11111,193 +11102,193 @@
       <c r="AH77" s="297"/>
     </row>
     <row r="78" spans="1:35" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="456" t="s">
+      <c r="A78" s="457" t="s">
         <v>75</v>
       </c>
-      <c r="B78" s="457"/>
-      <c r="C78" s="457"/>
-      <c r="D78" s="457"/>
-      <c r="E78" s="457"/>
-      <c r="F78" s="457"/>
-      <c r="G78" s="457"/>
-      <c r="H78" s="457"/>
-      <c r="I78" s="457"/>
-      <c r="J78" s="457"/>
-      <c r="K78" s="457"/>
-      <c r="L78" s="457"/>
-      <c r="M78" s="457"/>
-      <c r="N78" s="457"/>
-      <c r="O78" s="457"/>
-      <c r="P78" s="457"/>
-      <c r="Q78" s="457"/>
-      <c r="R78" s="457"/>
-      <c r="S78" s="457"/>
-      <c r="T78" s="457"/>
-      <c r="U78" s="457"/>
-      <c r="V78" s="457"/>
-      <c r="W78" s="457"/>
-      <c r="X78" s="457"/>
-      <c r="Y78" s="457"/>
-      <c r="Z78" s="457"/>
-      <c r="AA78" s="457"/>
-      <c r="AB78" s="457"/>
-      <c r="AC78" s="457"/>
-      <c r="AD78" s="457"/>
-      <c r="AE78" s="457"/>
-      <c r="AF78" s="457"/>
-      <c r="AG78" s="457"/>
-      <c r="AH78" s="458"/>
+      <c r="B78" s="458"/>
+      <c r="C78" s="458"/>
+      <c r="D78" s="458"/>
+      <c r="E78" s="458"/>
+      <c r="F78" s="458"/>
+      <c r="G78" s="458"/>
+      <c r="H78" s="458"/>
+      <c r="I78" s="458"/>
+      <c r="J78" s="458"/>
+      <c r="K78" s="458"/>
+      <c r="L78" s="458"/>
+      <c r="M78" s="458"/>
+      <c r="N78" s="458"/>
+      <c r="O78" s="458"/>
+      <c r="P78" s="458"/>
+      <c r="Q78" s="458"/>
+      <c r="R78" s="458"/>
+      <c r="S78" s="458"/>
+      <c r="T78" s="458"/>
+      <c r="U78" s="458"/>
+      <c r="V78" s="458"/>
+      <c r="W78" s="458"/>
+      <c r="X78" s="458"/>
+      <c r="Y78" s="458"/>
+      <c r="Z78" s="458"/>
+      <c r="AA78" s="458"/>
+      <c r="AB78" s="458"/>
+      <c r="AC78" s="458"/>
+      <c r="AD78" s="458"/>
+      <c r="AE78" s="458"/>
+      <c r="AF78" s="458"/>
+      <c r="AG78" s="458"/>
+      <c r="AH78" s="459"/>
     </row>
     <row r="79" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="450" t="s">
+      <c r="A79" s="451" t="s">
         <v>66</v>
       </c>
-      <c r="B79" s="451"/>
-      <c r="C79" s="451"/>
-      <c r="D79" s="451"/>
-      <c r="E79" s="451"/>
-      <c r="F79" s="451"/>
-      <c r="G79" s="451"/>
-      <c r="H79" s="451"/>
-      <c r="I79" s="451"/>
-      <c r="J79" s="451"/>
-      <c r="K79" s="451"/>
-      <c r="L79" s="452"/>
-      <c r="M79" s="10" t="s">
+      <c r="B79" s="452"/>
+      <c r="C79" s="452"/>
+      <c r="D79" s="452"/>
+      <c r="E79" s="452"/>
+      <c r="F79" s="452"/>
+      <c r="G79" s="452"/>
+      <c r="H79" s="452"/>
+      <c r="I79" s="452"/>
+      <c r="J79" s="452"/>
+      <c r="K79" s="452"/>
+      <c r="L79" s="453"/>
+      <c r="M79" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="N79" s="108" t="s">
+      <c r="N79" s="111" t="s">
         <v>67</v>
       </c>
-      <c r="O79" s="109"/>
-      <c r="P79" s="109"/>
-      <c r="Q79" s="109"/>
-      <c r="R79" s="109"/>
-      <c r="S79" s="109"/>
-      <c r="T79" s="109"/>
-      <c r="U79" s="109"/>
-      <c r="V79" s="109"/>
-      <c r="W79" s="109"/>
-      <c r="X79" s="109"/>
-      <c r="Y79" s="109"/>
-      <c r="Z79" s="109"/>
-      <c r="AA79" s="109"/>
-      <c r="AB79" s="109"/>
-      <c r="AC79" s="109"/>
-      <c r="AD79" s="109"/>
-      <c r="AE79" s="109"/>
-      <c r="AF79" s="109"/>
-      <c r="AG79" s="110"/>
-      <c r="AH79" s="10" t="s">
+      <c r="O79" s="112"/>
+      <c r="P79" s="112"/>
+      <c r="Q79" s="112"/>
+      <c r="R79" s="112"/>
+      <c r="S79" s="112"/>
+      <c r="T79" s="112"/>
+      <c r="U79" s="112"/>
+      <c r="V79" s="112"/>
+      <c r="W79" s="112"/>
+      <c r="X79" s="112"/>
+      <c r="Y79" s="112"/>
+      <c r="Z79" s="112"/>
+      <c r="AA79" s="112"/>
+      <c r="AB79" s="112"/>
+      <c r="AC79" s="112"/>
+      <c r="AD79" s="112"/>
+      <c r="AE79" s="112"/>
+      <c r="AF79" s="112"/>
+      <c r="AG79" s="113"/>
+      <c r="AH79" s="9" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="80" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="453" t="s">
+      <c r="A80" s="454" t="s">
         <v>71</v>
       </c>
-      <c r="B80" s="453"/>
-      <c r="C80" s="453"/>
-      <c r="D80" s="453"/>
-      <c r="E80" s="453"/>
-      <c r="F80" s="453"/>
-      <c r="G80" s="453"/>
-      <c r="H80" s="453"/>
-      <c r="I80" s="453"/>
-      <c r="J80" s="453"/>
-      <c r="K80" s="453"/>
-      <c r="L80" s="453"/>
-      <c r="M80" s="9" t="s">
+      <c r="B80" s="454"/>
+      <c r="C80" s="454"/>
+      <c r="D80" s="454"/>
+      <c r="E80" s="454"/>
+      <c r="F80" s="454"/>
+      <c r="G80" s="454"/>
+      <c r="H80" s="454"/>
+      <c r="I80" s="454"/>
+      <c r="J80" s="454"/>
+      <c r="K80" s="454"/>
+      <c r="L80" s="454"/>
+      <c r="M80" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="N80" s="111" t="s">
+      <c r="N80" s="114" t="s">
         <v>68</v>
       </c>
-      <c r="O80" s="112"/>
-      <c r="P80" s="112"/>
-      <c r="Q80" s="112"/>
-      <c r="R80" s="112"/>
-      <c r="S80" s="112"/>
-      <c r="T80" s="112"/>
-      <c r="U80" s="112"/>
-      <c r="V80" s="112"/>
-      <c r="W80" s="112"/>
-      <c r="X80" s="112"/>
-      <c r="Y80" s="112"/>
-      <c r="Z80" s="112"/>
-      <c r="AA80" s="112"/>
-      <c r="AB80" s="112"/>
-      <c r="AC80" s="112"/>
-      <c r="AD80" s="112"/>
-      <c r="AE80" s="112"/>
-      <c r="AF80" s="112"/>
-      <c r="AG80" s="113"/>
-      <c r="AH80" s="9" t="s">
+      <c r="O80" s="115"/>
+      <c r="P80" s="115"/>
+      <c r="Q80" s="115"/>
+      <c r="R80" s="115"/>
+      <c r="S80" s="115"/>
+      <c r="T80" s="115"/>
+      <c r="U80" s="115"/>
+      <c r="V80" s="115"/>
+      <c r="W80" s="115"/>
+      <c r="X80" s="115"/>
+      <c r="Y80" s="115"/>
+      <c r="Z80" s="115"/>
+      <c r="AA80" s="115"/>
+      <c r="AB80" s="115"/>
+      <c r="AC80" s="115"/>
+      <c r="AD80" s="115"/>
+      <c r="AE80" s="115"/>
+      <c r="AF80" s="115"/>
+      <c r="AG80" s="116"/>
+      <c r="AH80" s="8" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="81" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="453" t="s">
+      <c r="A81" s="454" t="s">
         <v>69</v>
       </c>
-      <c r="B81" s="453"/>
-      <c r="C81" s="453"/>
-      <c r="D81" s="453"/>
-      <c r="E81" s="453"/>
-      <c r="F81" s="453"/>
-      <c r="G81" s="453"/>
-      <c r="H81" s="453"/>
-      <c r="I81" s="453"/>
-      <c r="J81" s="453"/>
-      <c r="K81" s="453"/>
-      <c r="L81" s="453"/>
-      <c r="M81" s="9" t="s">
+      <c r="B81" s="454"/>
+      <c r="C81" s="454"/>
+      <c r="D81" s="454"/>
+      <c r="E81" s="454"/>
+      <c r="F81" s="454"/>
+      <c r="G81" s="454"/>
+      <c r="H81" s="454"/>
+      <c r="I81" s="454"/>
+      <c r="J81" s="454"/>
+      <c r="K81" s="454"/>
+      <c r="L81" s="454"/>
+      <c r="M81" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="N81" s="111" t="s">
+      <c r="N81" s="114" t="s">
         <v>73</v>
       </c>
-      <c r="O81" s="112"/>
-      <c r="P81" s="112"/>
-      <c r="Q81" s="112"/>
-      <c r="R81" s="112"/>
-      <c r="S81" s="112"/>
-      <c r="T81" s="112"/>
-      <c r="U81" s="112"/>
-      <c r="V81" s="112"/>
-      <c r="W81" s="112"/>
-      <c r="X81" s="112"/>
-      <c r="Y81" s="112"/>
-      <c r="Z81" s="112"/>
-      <c r="AA81" s="112"/>
-      <c r="AB81" s="112"/>
-      <c r="AC81" s="112"/>
-      <c r="AD81" s="112"/>
-      <c r="AE81" s="112"/>
-      <c r="AF81" s="112"/>
-      <c r="AG81" s="113"/>
-      <c r="AH81" s="9" t="s">
+      <c r="O81" s="115"/>
+      <c r="P81" s="115"/>
+      <c r="Q81" s="115"/>
+      <c r="R81" s="115"/>
+      <c r="S81" s="115"/>
+      <c r="T81" s="115"/>
+      <c r="U81" s="115"/>
+      <c r="V81" s="115"/>
+      <c r="W81" s="115"/>
+      <c r="X81" s="115"/>
+      <c r="Y81" s="115"/>
+      <c r="Z81" s="115"/>
+      <c r="AA81" s="115"/>
+      <c r="AB81" s="115"/>
+      <c r="AC81" s="115"/>
+      <c r="AD81" s="115"/>
+      <c r="AE81" s="115"/>
+      <c r="AF81" s="115"/>
+      <c r="AG81" s="116"/>
+      <c r="AH81" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="AI81" s="19"/>
-      <c r="AJ81" s="19"/>
+      <c r="AI81" s="18"/>
+      <c r="AJ81" s="18"/>
     </row>
     <row r="82" spans="1:36" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="454" t="s">
+      <c r="A82" s="455" t="s">
         <v>70</v>
       </c>
-      <c r="B82" s="455"/>
-      <c r="C82" s="455"/>
-      <c r="D82" s="455"/>
-      <c r="E82" s="455"/>
-      <c r="F82" s="455"/>
-      <c r="G82" s="455"/>
-      <c r="H82" s="455"/>
-      <c r="I82" s="455"/>
-      <c r="J82" s="455"/>
-      <c r="K82" s="455"/>
-      <c r="L82" s="455"/>
-      <c r="M82" s="9" t="s">
+      <c r="B82" s="456"/>
+      <c r="C82" s="456"/>
+      <c r="D82" s="456"/>
+      <c r="E82" s="456"/>
+      <c r="F82" s="456"/>
+      <c r="G82" s="456"/>
+      <c r="H82" s="456"/>
+      <c r="I82" s="456"/>
+      <c r="J82" s="456"/>
+      <c r="K82" s="456"/>
+      <c r="L82" s="456"/>
+      <c r="M82" s="8" t="s">
         <v>72</v>
       </c>
       <c r="N82" s="311" t="s">
@@ -11322,11 +11313,11 @@
       <c r="AE82" s="312"/>
       <c r="AF82" s="312"/>
       <c r="AG82" s="313"/>
-      <c r="AH82" s="11" t="s">
+      <c r="AH82" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="AI82" s="19"/>
-      <c r="AJ82" s="19"/>
+      <c r="AI82" s="18"/>
+      <c r="AJ82" s="18"/>
     </row>
     <row r="83" spans="1:36" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A83" s="291" t="s">
@@ -11367,124 +11358,124 @@
       <c r="AF83" s="293"/>
       <c r="AG83" s="293"/>
       <c r="AH83" s="294"/>
-      <c r="AI83" s="19"/>
-      <c r="AJ83" s="19"/>
+      <c r="AI83" s="18"/>
+      <c r="AJ83" s="18"/>
     </row>
     <row r="84" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="14"/>
-      <c r="B84" s="13"/>
-      <c r="C84" s="13"/>
-      <c r="D84" s="13"/>
-      <c r="E84" s="13"/>
-      <c r="F84" s="13"/>
-      <c r="G84" s="13"/>
-      <c r="H84" s="13"/>
-      <c r="I84" s="13"/>
-      <c r="J84" s="13"/>
-      <c r="K84" s="13"/>
-      <c r="L84" s="13"/>
-      <c r="M84" s="437" t="s">
+      <c r="A84" s="13"/>
+      <c r="B84" s="12"/>
+      <c r="C84" s="12"/>
+      <c r="D84" s="12"/>
+      <c r="E84" s="12"/>
+      <c r="F84" s="12"/>
+      <c r="G84" s="12"/>
+      <c r="H84" s="12"/>
+      <c r="I84" s="12"/>
+      <c r="J84" s="12"/>
+      <c r="K84" s="12"/>
+      <c r="L84" s="12"/>
+      <c r="M84" s="438" t="s">
         <v>78</v>
       </c>
-      <c r="N84" s="438"/>
-      <c r="O84" s="438"/>
-      <c r="P84" s="438"/>
-      <c r="Q84" s="438"/>
-      <c r="R84" s="438"/>
-      <c r="S84" s="438"/>
-      <c r="T84" s="438"/>
-      <c r="U84" s="438"/>
-      <c r="V84" s="438"/>
-      <c r="W84" s="438"/>
-      <c r="X84" s="438"/>
-      <c r="Y84" s="438"/>
-      <c r="Z84" s="438"/>
-      <c r="AA84" s="438"/>
-      <c r="AB84" s="438"/>
-      <c r="AC84" s="438"/>
-      <c r="AD84" s="438"/>
-      <c r="AE84" s="438"/>
-      <c r="AF84" s="438"/>
-      <c r="AG84" s="438"/>
-      <c r="AH84" s="439"/>
-      <c r="AI84" s="435"/>
-      <c r="AJ84" s="435"/>
+      <c r="N84" s="439"/>
+      <c r="O84" s="439"/>
+      <c r="P84" s="439"/>
+      <c r="Q84" s="439"/>
+      <c r="R84" s="439"/>
+      <c r="S84" s="439"/>
+      <c r="T84" s="439"/>
+      <c r="U84" s="439"/>
+      <c r="V84" s="439"/>
+      <c r="W84" s="439"/>
+      <c r="X84" s="439"/>
+      <c r="Y84" s="439"/>
+      <c r="Z84" s="439"/>
+      <c r="AA84" s="439"/>
+      <c r="AB84" s="439"/>
+      <c r="AC84" s="439"/>
+      <c r="AD84" s="439"/>
+      <c r="AE84" s="439"/>
+      <c r="AF84" s="439"/>
+      <c r="AG84" s="439"/>
+      <c r="AH84" s="440"/>
+      <c r="AI84" s="436"/>
+      <c r="AJ84" s="436"/>
     </row>
     <row r="85" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="15"/>
-      <c r="B85" s="16"/>
-      <c r="C85" s="16"/>
-      <c r="D85" s="16"/>
-      <c r="E85" s="16"/>
-      <c r="F85" s="16"/>
-      <c r="G85" s="16"/>
-      <c r="H85" s="16"/>
-      <c r="I85" s="16"/>
-      <c r="J85" s="16"/>
-      <c r="K85" s="16"/>
-      <c r="L85" s="16"/>
-      <c r="M85" s="440"/>
-      <c r="N85" s="441"/>
-      <c r="O85" s="441"/>
-      <c r="P85" s="441"/>
-      <c r="Q85" s="441"/>
-      <c r="R85" s="441"/>
-      <c r="S85" s="441"/>
-      <c r="T85" s="441"/>
-      <c r="U85" s="441"/>
-      <c r="V85" s="441"/>
-      <c r="W85" s="441"/>
-      <c r="X85" s="441"/>
-      <c r="Y85" s="441"/>
-      <c r="Z85" s="441"/>
-      <c r="AA85" s="441"/>
-      <c r="AB85" s="441"/>
-      <c r="AC85" s="441"/>
-      <c r="AD85" s="441"/>
-      <c r="AE85" s="441"/>
-      <c r="AF85" s="441"/>
-      <c r="AG85" s="441"/>
-      <c r="AH85" s="442"/>
-      <c r="AI85" s="20"/>
-      <c r="AJ85" s="20"/>
+      <c r="A85" s="14"/>
+      <c r="B85" s="15"/>
+      <c r="C85" s="15"/>
+      <c r="D85" s="15"/>
+      <c r="E85" s="15"/>
+      <c r="F85" s="15"/>
+      <c r="G85" s="15"/>
+      <c r="H85" s="15"/>
+      <c r="I85" s="15"/>
+      <c r="J85" s="15"/>
+      <c r="K85" s="15"/>
+      <c r="L85" s="15"/>
+      <c r="M85" s="441"/>
+      <c r="N85" s="442"/>
+      <c r="O85" s="442"/>
+      <c r="P85" s="442"/>
+      <c r="Q85" s="442"/>
+      <c r="R85" s="442"/>
+      <c r="S85" s="442"/>
+      <c r="T85" s="442"/>
+      <c r="U85" s="442"/>
+      <c r="V85" s="442"/>
+      <c r="W85" s="442"/>
+      <c r="X85" s="442"/>
+      <c r="Y85" s="442"/>
+      <c r="Z85" s="442"/>
+      <c r="AA85" s="442"/>
+      <c r="AB85" s="442"/>
+      <c r="AC85" s="442"/>
+      <c r="AD85" s="442"/>
+      <c r="AE85" s="442"/>
+      <c r="AF85" s="442"/>
+      <c r="AG85" s="442"/>
+      <c r="AH85" s="443"/>
+      <c r="AI85" s="19"/>
+      <c r="AJ85" s="19"/>
     </row>
     <row r="86" spans="1:36" ht="135" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="18"/>
-      <c r="B86" s="17"/>
-      <c r="C86" s="17"/>
-      <c r="D86" s="17"/>
-      <c r="E86" s="17"/>
-      <c r="F86" s="17"/>
-      <c r="G86" s="17"/>
-      <c r="H86" s="17"/>
-      <c r="I86" s="17"/>
-      <c r="J86" s="17"/>
-      <c r="K86" s="17"/>
-      <c r="L86" s="17"/>
-      <c r="M86" s="443"/>
-      <c r="N86" s="444"/>
-      <c r="O86" s="444"/>
-      <c r="P86" s="444"/>
-      <c r="Q86" s="444"/>
-      <c r="R86" s="444"/>
-      <c r="S86" s="444"/>
-      <c r="T86" s="444"/>
-      <c r="U86" s="444"/>
-      <c r="V86" s="444"/>
-      <c r="W86" s="444"/>
-      <c r="X86" s="444"/>
-      <c r="Y86" s="444"/>
-      <c r="Z86" s="444"/>
-      <c r="AA86" s="444"/>
-      <c r="AB86" s="444"/>
-      <c r="AC86" s="444"/>
-      <c r="AD86" s="444"/>
-      <c r="AE86" s="444"/>
-      <c r="AF86" s="444"/>
-      <c r="AG86" s="444"/>
-      <c r="AH86" s="445"/>
-      <c r="AI86" s="436"/>
-      <c r="AJ86" s="436"/>
+      <c r="A86" s="17"/>
+      <c r="B86" s="16"/>
+      <c r="C86" s="16"/>
+      <c r="D86" s="16"/>
+      <c r="E86" s="16"/>
+      <c r="F86" s="16"/>
+      <c r="G86" s="16"/>
+      <c r="H86" s="16"/>
+      <c r="I86" s="16"/>
+      <c r="J86" s="16"/>
+      <c r="K86" s="16"/>
+      <c r="L86" s="16"/>
+      <c r="M86" s="444"/>
+      <c r="N86" s="445"/>
+      <c r="O86" s="445"/>
+      <c r="P86" s="445"/>
+      <c r="Q86" s="445"/>
+      <c r="R86" s="445"/>
+      <c r="S86" s="445"/>
+      <c r="T86" s="445"/>
+      <c r="U86" s="445"/>
+      <c r="V86" s="445"/>
+      <c r="W86" s="445"/>
+      <c r="X86" s="445"/>
+      <c r="Y86" s="445"/>
+      <c r="Z86" s="445"/>
+      <c r="AA86" s="445"/>
+      <c r="AB86" s="445"/>
+      <c r="AC86" s="445"/>
+      <c r="AD86" s="445"/>
+      <c r="AE86" s="445"/>
+      <c r="AF86" s="445"/>
+      <c r="AG86" s="445"/>
+      <c r="AH86" s="446"/>
+      <c r="AI86" s="437"/>
+      <c r="AJ86" s="437"/>
     </row>
     <row r="87" spans="1:36" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A87" s="345" t="s">
@@ -11525,40 +11516,40 @@
       <c r="AH87" s="348"/>
     </row>
     <row r="88" spans="1:36" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="21"/>
-      <c r="B88" s="21"/>
-      <c r="C88" s="21"/>
-      <c r="D88" s="21"/>
-      <c r="E88" s="21"/>
-      <c r="F88" s="21"/>
-      <c r="G88" s="21"/>
-      <c r="H88" s="21"/>
-      <c r="I88" s="21"/>
-      <c r="J88" s="21"/>
-      <c r="K88" s="21"/>
-      <c r="L88" s="21"/>
-      <c r="M88" s="21"/>
-      <c r="N88" s="21"/>
-      <c r="O88" s="21"/>
-      <c r="P88" s="21"/>
-      <c r="Q88" s="21"/>
-      <c r="R88" s="21"/>
-      <c r="S88" s="21"/>
-      <c r="T88" s="21"/>
-      <c r="U88" s="21"/>
-      <c r="V88" s="21"/>
-      <c r="W88" s="21"/>
-      <c r="X88" s="21"/>
-      <c r="Y88" s="21"/>
-      <c r="Z88" s="21"/>
-      <c r="AA88" s="21"/>
-      <c r="AB88" s="21"/>
-      <c r="AC88" s="21"/>
-      <c r="AD88" s="21"/>
-      <c r="AE88" s="21"/>
-      <c r="AF88" s="21"/>
-      <c r="AG88" s="21"/>
-      <c r="AH88" s="30"/>
+      <c r="A88" s="20"/>
+      <c r="B88" s="20"/>
+      <c r="C88" s="20"/>
+      <c r="D88" s="20"/>
+      <c r="E88" s="20"/>
+      <c r="F88" s="20"/>
+      <c r="G88" s="20"/>
+      <c r="H88" s="20"/>
+      <c r="I88" s="20"/>
+      <c r="J88" s="20"/>
+      <c r="K88" s="20"/>
+      <c r="L88" s="20"/>
+      <c r="M88" s="20"/>
+      <c r="N88" s="20"/>
+      <c r="O88" s="20"/>
+      <c r="P88" s="20"/>
+      <c r="Q88" s="20"/>
+      <c r="R88" s="20"/>
+      <c r="S88" s="20"/>
+      <c r="T88" s="20"/>
+      <c r="U88" s="20"/>
+      <c r="V88" s="20"/>
+      <c r="W88" s="20"/>
+      <c r="X88" s="20"/>
+      <c r="Y88" s="20"/>
+      <c r="Z88" s="20"/>
+      <c r="AA88" s="20"/>
+      <c r="AB88" s="20"/>
+      <c r="AC88" s="20"/>
+      <c r="AD88" s="20"/>
+      <c r="AE88" s="20"/>
+      <c r="AF88" s="20"/>
+      <c r="AG88" s="20"/>
+      <c r="AH88" s="27"/>
     </row>
     <row r="89" spans="1:36" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A89" s="291" t="s">
@@ -12065,10 +12056,10 @@
       <c r="AH101" s="401"/>
     </row>
     <row r="102" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="5" t="s">
+      <c r="A102" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="AH102" s="6"/>
+      <c r="AH102" s="5"/>
     </row>
     <row r="103" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="422" t="s">
@@ -12216,8 +12207,8 @@
       <c r="AC107" s="405"/>
       <c r="AD107" s="405"/>
       <c r="AE107" s="405"/>
-      <c r="AF107" s="33"/>
-      <c r="AG107" s="33"/>
+      <c r="AF107" s="30"/>
+      <c r="AG107" s="30"/>
     </row>
     <row r="108" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A108" s="405"/>
@@ -12251,8 +12242,8 @@
       <c r="AC108" s="405"/>
       <c r="AD108" s="405"/>
       <c r="AE108" s="405"/>
-      <c r="AF108" s="33"/>
-      <c r="AG108" s="33"/>
+      <c r="AF108" s="30"/>
+      <c r="AG108" s="30"/>
     </row>
     <row r="109" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A109" s="405"/>
@@ -12286,8 +12277,8 @@
       <c r="AC109" s="405"/>
       <c r="AD109" s="405"/>
       <c r="AE109" s="405"/>
-      <c r="AF109" s="33"/>
-      <c r="AG109" s="33"/>
+      <c r="AF109" s="30"/>
+      <c r="AG109" s="30"/>
     </row>
     <row r="110" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A110" s="405"/>
@@ -12321,8 +12312,8 @@
       <c r="AC110" s="405"/>
       <c r="AD110" s="405"/>
       <c r="AE110" s="405"/>
-      <c r="AF110" s="33"/>
-      <c r="AG110" s="33"/>
+      <c r="AF110" s="30"/>
+      <c r="AG110" s="30"/>
     </row>
     <row r="111" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A111" s="405"/>
@@ -12356,8 +12347,8 @@
       <c r="AC111" s="405"/>
       <c r="AD111" s="405"/>
       <c r="AE111" s="405"/>
-      <c r="AF111" s="33"/>
-      <c r="AG111" s="33"/>
+      <c r="AF111" s="30"/>
+      <c r="AG111" s="30"/>
     </row>
     <row r="112" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A112" s="405"/>
@@ -12391,8 +12382,8 @@
       <c r="AC112" s="405"/>
       <c r="AD112" s="405"/>
       <c r="AE112" s="405"/>
-      <c r="AF112" s="33"/>
-      <c r="AG112" s="33"/>
+      <c r="AF112" s="30"/>
+      <c r="AG112" s="30"/>
     </row>
     <row r="113" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A113" s="405"/>
@@ -12426,8 +12417,8 @@
       <c r="AC113" s="405"/>
       <c r="AD113" s="405"/>
       <c r="AE113" s="405"/>
-      <c r="AF113" s="33"/>
-      <c r="AG113" s="33"/>
+      <c r="AF113" s="30"/>
+      <c r="AG113" s="30"/>
     </row>
     <row r="114" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A114" s="405"/>
@@ -12461,8 +12452,8 @@
       <c r="AC114" s="405"/>
       <c r="AD114" s="405"/>
       <c r="AE114" s="405"/>
-      <c r="AF114" s="33"/>
-      <c r="AG114" s="33"/>
+      <c r="AF114" s="30"/>
+      <c r="AG114" s="30"/>
     </row>
     <row r="115" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A115" s="405"/>
@@ -12496,8 +12487,8 @@
       <c r="AC115" s="405"/>
       <c r="AD115" s="405"/>
       <c r="AE115" s="405"/>
-      <c r="AF115" s="33"/>
-      <c r="AG115" s="33"/>
+      <c r="AF115" s="30"/>
+      <c r="AG115" s="30"/>
     </row>
     <row r="116" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A116" s="405"/>
@@ -12531,8 +12522,8 @@
       <c r="AC116" s="405"/>
       <c r="AD116" s="405"/>
       <c r="AE116" s="405"/>
-      <c r="AF116" s="33"/>
-      <c r="AG116" s="33"/>
+      <c r="AF116" s="30"/>
+      <c r="AG116" s="30"/>
     </row>
     <row r="117" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A117" s="405"/>
@@ -12566,8 +12557,8 @@
       <c r="AC117" s="405"/>
       <c r="AD117" s="405"/>
       <c r="AE117" s="405"/>
-      <c r="AF117" s="33"/>
-      <c r="AG117" s="33"/>
+      <c r="AF117" s="30"/>
+      <c r="AG117" s="30"/>
     </row>
     <row r="118" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A118" s="405"/>
@@ -12601,8 +12592,8 @@
       <c r="AC118" s="405"/>
       <c r="AD118" s="405"/>
       <c r="AE118" s="405"/>
-      <c r="AF118" s="33"/>
-      <c r="AG118" s="33"/>
+      <c r="AF118" s="30"/>
+      <c r="AG118" s="30"/>
     </row>
     <row r="119" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A119" s="405"/>
@@ -12636,8 +12627,8 @@
       <c r="AC119" s="405"/>
       <c r="AD119" s="405"/>
       <c r="AE119" s="405"/>
-      <c r="AF119" s="33"/>
-      <c r="AG119" s="33"/>
+      <c r="AF119" s="30"/>
+      <c r="AG119" s="30"/>
     </row>
     <row r="120" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A120" s="405"/>
@@ -12671,8 +12662,8 @@
       <c r="AC120" s="405"/>
       <c r="AD120" s="405"/>
       <c r="AE120" s="405"/>
-      <c r="AF120" s="33"/>
-      <c r="AG120" s="33"/>
+      <c r="AF120" s="30"/>
+      <c r="AG120" s="30"/>
     </row>
     <row r="121" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A121" s="405"/>
@@ -12706,8 +12697,8 @@
       <c r="AC121" s="405"/>
       <c r="AD121" s="405"/>
       <c r="AE121" s="405"/>
-      <c r="AF121" s="33"/>
-      <c r="AG121" s="33"/>
+      <c r="AF121" s="30"/>
+      <c r="AG121" s="30"/>
     </row>
     <row r="122" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A122" s="405"/>
@@ -12741,8 +12732,8 @@
       <c r="AC122" s="405"/>
       <c r="AD122" s="405"/>
       <c r="AE122" s="405"/>
-      <c r="AF122" s="33"/>
-      <c r="AG122" s="33"/>
+      <c r="AF122" s="30"/>
+      <c r="AG122" s="30"/>
     </row>
     <row r="123" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A123" s="405"/>
@@ -12776,8 +12767,8 @@
       <c r="AC123" s="405"/>
       <c r="AD123" s="405"/>
       <c r="AE123" s="405"/>
-      <c r="AF123" s="33"/>
-      <c r="AG123" s="33"/>
+      <c r="AF123" s="30"/>
+      <c r="AG123" s="30"/>
     </row>
     <row r="124" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A124" s="405"/>
@@ -12811,8 +12802,8 @@
       <c r="AC124" s="405"/>
       <c r="AD124" s="405"/>
       <c r="AE124" s="405"/>
-      <c r="AF124" s="33"/>
-      <c r="AG124" s="33"/>
+      <c r="AF124" s="30"/>
+      <c r="AG124" s="30"/>
     </row>
     <row r="125" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A125" s="405"/>
@@ -12846,8 +12837,8 @@
       <c r="AC125" s="405"/>
       <c r="AD125" s="405"/>
       <c r="AE125" s="405"/>
-      <c r="AF125" s="33"/>
-      <c r="AG125" s="33"/>
+      <c r="AF125" s="30"/>
+      <c r="AG125" s="30"/>
     </row>
     <row r="126" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A126" s="405"/>
@@ -12881,8 +12872,8 @@
       <c r="AC126" s="405"/>
       <c r="AD126" s="405"/>
       <c r="AE126" s="405"/>
-      <c r="AF126" s="33"/>
-      <c r="AG126" s="33"/>
+      <c r="AF126" s="30"/>
+      <c r="AG126" s="30"/>
     </row>
     <row r="127" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A127" s="405"/>
@@ -12916,8 +12907,8 @@
       <c r="AC127" s="405"/>
       <c r="AD127" s="405"/>
       <c r="AE127" s="405"/>
-      <c r="AF127" s="33"/>
-      <c r="AG127" s="33"/>
+      <c r="AF127" s="30"/>
+      <c r="AG127" s="30"/>
     </row>
     <row r="128" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A128" s="405"/>
@@ -12951,8 +12942,8 @@
       <c r="AC128" s="405"/>
       <c r="AD128" s="405"/>
       <c r="AE128" s="405"/>
-      <c r="AF128" s="33"/>
-      <c r="AG128" s="33"/>
+      <c r="AF128" s="30"/>
+      <c r="AG128" s="30"/>
     </row>
     <row r="129" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A129" s="405"/>
@@ -12986,8 +12977,8 @@
       <c r="AC129" s="405"/>
       <c r="AD129" s="405"/>
       <c r="AE129" s="405"/>
-      <c r="AF129" s="33"/>
-      <c r="AG129" s="33"/>
+      <c r="AF129" s="30"/>
+      <c r="AG129" s="30"/>
     </row>
     <row r="130" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A130" s="405"/>
@@ -13021,8 +13012,8 @@
       <c r="AC130" s="405"/>
       <c r="AD130" s="405"/>
       <c r="AE130" s="405"/>
-      <c r="AF130" s="33"/>
-      <c r="AG130" s="33"/>
+      <c r="AF130" s="30"/>
+      <c r="AG130" s="30"/>
     </row>
     <row r="131" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A131" s="405"/>
@@ -13056,8 +13047,8 @@
       <c r="AC131" s="405"/>
       <c r="AD131" s="405"/>
       <c r="AE131" s="405"/>
-      <c r="AF131" s="33"/>
-      <c r="AG131" s="33"/>
+      <c r="AF131" s="30"/>
+      <c r="AG131" s="30"/>
     </row>
     <row r="132" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A132" s="405"/>
@@ -13091,8 +13082,8 @@
       <c r="AC132" s="405"/>
       <c r="AD132" s="405"/>
       <c r="AE132" s="405"/>
-      <c r="AF132" s="33"/>
-      <c r="AG132" s="33"/>
+      <c r="AF132" s="30"/>
+      <c r="AG132" s="30"/>
     </row>
     <row r="133" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A133" s="405"/>
@@ -13126,8 +13117,8 @@
       <c r="AC133" s="405"/>
       <c r="AD133" s="405"/>
       <c r="AE133" s="405"/>
-      <c r="AF133" s="33"/>
-      <c r="AG133" s="33"/>
+      <c r="AF133" s="30"/>
+      <c r="AG133" s="30"/>
     </row>
     <row r="134" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A134" s="405"/>
@@ -13161,8 +13152,8 @@
       <c r="AC134" s="405"/>
       <c r="AD134" s="405"/>
       <c r="AE134" s="405"/>
-      <c r="AF134" s="33"/>
-      <c r="AG134" s="33"/>
+      <c r="AF134" s="30"/>
+      <c r="AG134" s="30"/>
     </row>
     <row r="135" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A135" s="405"/>
@@ -13196,8 +13187,8 @@
       <c r="AC135" s="405"/>
       <c r="AD135" s="405"/>
       <c r="AE135" s="405"/>
-      <c r="AF135" s="33"/>
-      <c r="AG135" s="33"/>
+      <c r="AF135" s="30"/>
+      <c r="AG135" s="30"/>
     </row>
     <row r="136" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A136" s="405"/>
@@ -13231,8 +13222,8 @@
       <c r="AC136" s="405"/>
       <c r="AD136" s="405"/>
       <c r="AE136" s="405"/>
-      <c r="AF136" s="33"/>
-      <c r="AG136" s="33"/>
+      <c r="AF136" s="30"/>
+      <c r="AG136" s="30"/>
     </row>
     <row r="137" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A137" s="405"/>
@@ -13266,8 +13257,8 @@
       <c r="AC137" s="405"/>
       <c r="AD137" s="405"/>
       <c r="AE137" s="405"/>
-      <c r="AF137" s="33"/>
-      <c r="AG137" s="33"/>
+      <c r="AF137" s="30"/>
+      <c r="AG137" s="30"/>
     </row>
     <row r="138" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A138" s="405"/>
@@ -13301,8 +13292,8 @@
       <c r="AC138" s="405"/>
       <c r="AD138" s="405"/>
       <c r="AE138" s="405"/>
-      <c r="AF138" s="33"/>
-      <c r="AG138" s="33"/>
+      <c r="AF138" s="30"/>
+      <c r="AG138" s="30"/>
     </row>
     <row r="139" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A139" s="405"/>
@@ -13336,8 +13327,8 @@
       <c r="AC139" s="405"/>
       <c r="AD139" s="405"/>
       <c r="AE139" s="405"/>
-      <c r="AF139" s="33"/>
-      <c r="AG139" s="33"/>
+      <c r="AF139" s="30"/>
+      <c r="AG139" s="30"/>
     </row>
     <row r="140" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A140" s="405"/>
@@ -13371,8 +13362,8 @@
       <c r="AC140" s="405"/>
       <c r="AD140" s="405"/>
       <c r="AE140" s="405"/>
-      <c r="AF140" s="33"/>
-      <c r="AG140" s="33"/>
+      <c r="AF140" s="30"/>
+      <c r="AG140" s="30"/>
     </row>
     <row r="141" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A141" s="405"/>
@@ -13406,8 +13397,8 @@
       <c r="AC141" s="405"/>
       <c r="AD141" s="405"/>
       <c r="AE141" s="405"/>
-      <c r="AF141" s="33"/>
-      <c r="AG141" s="33"/>
+      <c r="AF141" s="30"/>
+      <c r="AG141" s="30"/>
     </row>
     <row r="142" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A142" s="405"/>
@@ -13441,8 +13432,8 @@
       <c r="AC142" s="405"/>
       <c r="AD142" s="405"/>
       <c r="AE142" s="405"/>
-      <c r="AF142" s="33"/>
-      <c r="AG142" s="33"/>
+      <c r="AF142" s="30"/>
+      <c r="AG142" s="30"/>
     </row>
     <row r="143" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A143" s="405"/>
@@ -13476,8 +13467,8 @@
       <c r="AC143" s="405"/>
       <c r="AD143" s="405"/>
       <c r="AE143" s="405"/>
-      <c r="AF143" s="33"/>
-      <c r="AG143" s="33"/>
+      <c r="AF143" s="30"/>
+      <c r="AG143" s="30"/>
     </row>
     <row r="144" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A144" s="405"/>
@@ -13511,8 +13502,8 @@
       <c r="AC144" s="405"/>
       <c r="AD144" s="405"/>
       <c r="AE144" s="405"/>
-      <c r="AF144" s="33"/>
-      <c r="AG144" s="33"/>
+      <c r="AF144" s="30"/>
+      <c r="AG144" s="30"/>
     </row>
     <row r="145" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A145" s="405"/>
@@ -13546,8 +13537,8 @@
       <c r="AC145" s="405"/>
       <c r="AD145" s="405"/>
       <c r="AE145" s="405"/>
-      <c r="AF145" s="33"/>
-      <c r="AG145" s="33"/>
+      <c r="AF145" s="30"/>
+      <c r="AG145" s="30"/>
     </row>
     <row r="146" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A146" s="405"/>
@@ -13581,8 +13572,8 @@
       <c r="AC146" s="405"/>
       <c r="AD146" s="405"/>
       <c r="AE146" s="405"/>
-      <c r="AF146" s="33"/>
-      <c r="AG146" s="33"/>
+      <c r="AF146" s="30"/>
+      <c r="AG146" s="30"/>
     </row>
     <row r="147" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A147" s="405"/>
@@ -13616,8 +13607,8 @@
       <c r="AC147" s="405"/>
       <c r="AD147" s="405"/>
       <c r="AE147" s="405"/>
-      <c r="AF147" s="33"/>
-      <c r="AG147" s="33"/>
+      <c r="AF147" s="30"/>
+      <c r="AG147" s="30"/>
     </row>
     <row r="148" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A148" s="405"/>
@@ -13651,8 +13642,8 @@
       <c r="AC148" s="405"/>
       <c r="AD148" s="405"/>
       <c r="AE148" s="405"/>
-      <c r="AF148" s="33"/>
-      <c r="AG148" s="33"/>
+      <c r="AF148" s="30"/>
+      <c r="AG148" s="30"/>
     </row>
     <row r="149" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A149" s="405"/>
@@ -13686,8 +13677,8 @@
       <c r="AC149" s="405"/>
       <c r="AD149" s="405"/>
       <c r="AE149" s="405"/>
-      <c r="AF149" s="33"/>
-      <c r="AG149" s="33"/>
+      <c r="AF149" s="30"/>
+      <c r="AG149" s="30"/>
     </row>
     <row r="150" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A150" s="405"/>
@@ -13721,8 +13712,8 @@
       <c r="AC150" s="405"/>
       <c r="AD150" s="405"/>
       <c r="AE150" s="405"/>
-      <c r="AF150" s="33"/>
-      <c r="AG150" s="33"/>
+      <c r="AF150" s="30"/>
+      <c r="AG150" s="30"/>
     </row>
     <row r="151" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A151" s="405"/>
@@ -13756,8 +13747,8 @@
       <c r="AC151" s="405"/>
       <c r="AD151" s="405"/>
       <c r="AE151" s="405"/>
-      <c r="AF151" s="33"/>
-      <c r="AG151" s="33"/>
+      <c r="AF151" s="30"/>
+      <c r="AG151" s="30"/>
     </row>
     <row r="152" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A152" s="405"/>
@@ -13791,8 +13782,8 @@
       <c r="AC152" s="405"/>
       <c r="AD152" s="405"/>
       <c r="AE152" s="405"/>
-      <c r="AF152" s="33"/>
-      <c r="AG152" s="33"/>
+      <c r="AF152" s="30"/>
+      <c r="AG152" s="30"/>
     </row>
     <row r="153" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A153" s="405"/>
@@ -13826,8 +13817,8 @@
       <c r="AC153" s="405"/>
       <c r="AD153" s="405"/>
       <c r="AE153" s="405"/>
-      <c r="AF153" s="33"/>
-      <c r="AG153" s="33"/>
+      <c r="AF153" s="30"/>
+      <c r="AG153" s="30"/>
     </row>
     <row r="154" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A154" s="405"/>
@@ -13861,8 +13852,8 @@
       <c r="AC154" s="405"/>
       <c r="AD154" s="405"/>
       <c r="AE154" s="405"/>
-      <c r="AF154" s="33"/>
-      <c r="AG154" s="33"/>
+      <c r="AF154" s="30"/>
+      <c r="AG154" s="30"/>
     </row>
     <row r="155" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A155" s="405"/>
@@ -13896,8 +13887,8 @@
       <c r="AC155" s="405"/>
       <c r="AD155" s="405"/>
       <c r="AE155" s="405"/>
-      <c r="AF155" s="33"/>
-      <c r="AG155" s="33"/>
+      <c r="AF155" s="30"/>
+      <c r="AG155" s="30"/>
     </row>
     <row r="156" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A156" s="405"/>
@@ -13931,8 +13922,8 @@
       <c r="AC156" s="405"/>
       <c r="AD156" s="405"/>
       <c r="AE156" s="405"/>
-      <c r="AF156" s="33"/>
-      <c r="AG156" s="33"/>
+      <c r="AF156" s="30"/>
+      <c r="AG156" s="30"/>
     </row>
     <row r="157" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A157" s="405"/>
@@ -13966,8 +13957,8 @@
       <c r="AC157" s="405"/>
       <c r="AD157" s="405"/>
       <c r="AE157" s="405"/>
-      <c r="AF157" s="33"/>
-      <c r="AG157" s="33"/>
+      <c r="AF157" s="30"/>
+      <c r="AG157" s="30"/>
     </row>
     <row r="158" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A158" s="405"/>
@@ -14001,8 +13992,8 @@
       <c r="AC158" s="405"/>
       <c r="AD158" s="405"/>
       <c r="AE158" s="405"/>
-      <c r="AF158" s="33"/>
-      <c r="AG158" s="33"/>
+      <c r="AF158" s="30"/>
+      <c r="AG158" s="30"/>
     </row>
     <row r="159" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A159" s="405"/>
@@ -14036,8 +14027,8 @@
       <c r="AC159" s="405"/>
       <c r="AD159" s="405"/>
       <c r="AE159" s="405"/>
-      <c r="AF159" s="33"/>
-      <c r="AG159" s="33"/>
+      <c r="AF159" s="30"/>
+      <c r="AG159" s="30"/>
     </row>
     <row r="160" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A160" s="405"/>
@@ -14071,8 +14062,8 @@
       <c r="AC160" s="405"/>
       <c r="AD160" s="405"/>
       <c r="AE160" s="405"/>
-      <c r="AF160" s="33"/>
-      <c r="AG160" s="33"/>
+      <c r="AF160" s="30"/>
+      <c r="AG160" s="30"/>
     </row>
     <row r="161" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A161" s="405"/>
@@ -14106,8 +14097,8 @@
       <c r="AC161" s="405"/>
       <c r="AD161" s="405"/>
       <c r="AE161" s="405"/>
-      <c r="AF161" s="33"/>
-      <c r="AG161" s="33"/>
+      <c r="AF161" s="30"/>
+      <c r="AG161" s="30"/>
     </row>
     <row r="162" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A162" s="405"/>
@@ -14141,8 +14132,8 @@
       <c r="AC162" s="405"/>
       <c r="AD162" s="405"/>
       <c r="AE162" s="405"/>
-      <c r="AF162" s="33"/>
-      <c r="AG162" s="33"/>
+      <c r="AF162" s="30"/>
+      <c r="AG162" s="30"/>
     </row>
     <row r="163" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A163" s="405"/>
@@ -14176,8 +14167,8 @@
       <c r="AC163" s="405"/>
       <c r="AD163" s="405"/>
       <c r="AE163" s="405"/>
-      <c r="AF163" s="33"/>
-      <c r="AG163" s="33"/>
+      <c r="AF163" s="30"/>
+      <c r="AG163" s="30"/>
     </row>
     <row r="164" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A164" s="405"/>
@@ -14211,8 +14202,8 @@
       <c r="AC164" s="405"/>
       <c r="AD164" s="405"/>
       <c r="AE164" s="405"/>
-      <c r="AF164" s="33"/>
-      <c r="AG164" s="33"/>
+      <c r="AF164" s="30"/>
+      <c r="AG164" s="30"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
@@ -14297,7 +14288,7 @@
     <protectedRange sqref="A48:AH49" name="Rango76"/>
     <protectedRange sqref="A72:XFD72" name="Rango78"/>
   </protectedRanges>
-  <mergeCells count="380">
+  <mergeCells count="381">
     <mergeCell ref="G37:L37"/>
     <mergeCell ref="G38:L38"/>
     <mergeCell ref="N7:P7"/>
@@ -14331,6 +14322,21 @@
     <mergeCell ref="A160:AE160"/>
     <mergeCell ref="A161:AE161"/>
     <mergeCell ref="A162:AE162"/>
+    <mergeCell ref="A134:AE134"/>
+    <mergeCell ref="A135:AE135"/>
+    <mergeCell ref="A136:AE136"/>
+    <mergeCell ref="A137:AE137"/>
+    <mergeCell ref="A138:AE138"/>
+    <mergeCell ref="A139:AE139"/>
+    <mergeCell ref="A122:AE122"/>
+    <mergeCell ref="A123:AE123"/>
+    <mergeCell ref="A124:AE124"/>
+    <mergeCell ref="A125:AE125"/>
+    <mergeCell ref="A126:AE126"/>
+    <mergeCell ref="A127:AE127"/>
+    <mergeCell ref="A128:AE128"/>
+    <mergeCell ref="A129:AE129"/>
+    <mergeCell ref="A130:AE130"/>
     <mergeCell ref="A163:AE163"/>
     <mergeCell ref="A164:AE164"/>
     <mergeCell ref="G39:L39"/>
@@ -14355,21 +14361,6 @@
     <mergeCell ref="A131:AE131"/>
     <mergeCell ref="A132:AE132"/>
     <mergeCell ref="A133:AE133"/>
-    <mergeCell ref="A134:AE134"/>
-    <mergeCell ref="A135:AE135"/>
-    <mergeCell ref="A136:AE136"/>
-    <mergeCell ref="A137:AE137"/>
-    <mergeCell ref="A138:AE138"/>
-    <mergeCell ref="A139:AE139"/>
-    <mergeCell ref="A122:AE122"/>
-    <mergeCell ref="A123:AE123"/>
-    <mergeCell ref="A124:AE124"/>
-    <mergeCell ref="A125:AE125"/>
-    <mergeCell ref="A126:AE126"/>
-    <mergeCell ref="A127:AE127"/>
-    <mergeCell ref="A128:AE128"/>
-    <mergeCell ref="A129:AE129"/>
-    <mergeCell ref="A130:AE130"/>
     <mergeCell ref="A113:AE113"/>
     <mergeCell ref="A114:AE114"/>
     <mergeCell ref="A115:AE115"/>
@@ -14678,9 +14669,10 @@
     <mergeCell ref="AE21:AF21"/>
     <mergeCell ref="AE22:AF22"/>
     <mergeCell ref="AG21:AH21"/>
+    <mergeCell ref="AB42:AD42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="55" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="53" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <rowBreaks count="2" manualBreakCount="2">
     <brk id="58" max="33" man="1"/>
     <brk id="87" max="31" man="1"/>
@@ -14901,7 +14893,7 @@
                   </from>
                   <to>
                     <xdr:col>10</xdr:col>
-                    <xdr:colOff>514350</xdr:colOff>
+                    <xdr:colOff>495300</xdr:colOff>
                     <xdr:row>14</xdr:row>
                     <xdr:rowOff>95250</xdr:rowOff>
                   </to>
@@ -15011,7 +15003,7 @@
                   </from>
                   <to>
                     <xdr:col>10</xdr:col>
-                    <xdr:colOff>38100</xdr:colOff>
+                    <xdr:colOff>19050</xdr:colOff>
                     <xdr:row>51</xdr:row>
                     <xdr:rowOff>47625</xdr:rowOff>
                   </to>
@@ -15055,7 +15047,7 @@
                   </from>
                   <to>
                     <xdr:col>10</xdr:col>
-                    <xdr:colOff>19050</xdr:colOff>
+                    <xdr:colOff>0</xdr:colOff>
                     <xdr:row>52</xdr:row>
                     <xdr:rowOff>114300</xdr:rowOff>
                   </to>
@@ -15186,8 +15178,8 @@
                     <xdr:rowOff>209550</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>13</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>12</xdr:col>
+                    <xdr:colOff>495300</xdr:colOff>
                     <xdr:row>55</xdr:row>
                     <xdr:rowOff>123825</xdr:rowOff>
                   </to>
@@ -15318,8 +15310,8 @@
                     <xdr:rowOff>171450</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>13</xdr:col>
-                    <xdr:colOff>57150</xdr:colOff>
+                    <xdr:col>12</xdr:col>
+                    <xdr:colOff>552450</xdr:colOff>
                     <xdr:row>57</xdr:row>
                     <xdr:rowOff>133350</xdr:rowOff>
                   </to>

</xml_diff>